<commit_message>
Add parsing XLS(X) with ConditionalOverlay
</commit_message>
<xml_diff>
--- a/tests/assets/oca_template.xlsx
+++ b/tests/assets/oca_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="READ ME" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="188">
   <si>
     <t xml:space="preserve">OCA DATA CAPTURE SPECIFICATION</t>
   </si>
@@ -806,6 +806,12 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">OL: Conditional [Condition]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OL: Conditional [Dependencies]</t>
+  </si>
+  <si>
     <t xml:space="preserve">projectName</t>
   </si>
   <si>
@@ -857,6 +863,28 @@
     <t xml:space="preserve">linkedForm</t>
   </si>
   <si>
+    <t xml:space="preserve">${0}==‘LEI’ || ${1}==‘SHAP’</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">legalEntityType,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">programmeType</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">SDG_goal</t>
   </si>
   <si>
@@ -1002,6 +1030,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">元 </t>
     </r>
@@ -1021,6 +1050,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">表格名称</t>
     </r>
@@ -1052,6 +1082,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">元 </t>
     </r>
@@ -1071,6 +1102,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">表格说明</t>
     </r>
@@ -1102,6 +1134,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">属性名</t>
     </r>
@@ -1123,6 +1156,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">标签</t>
     </r>
@@ -1144,6 +1178,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">条目</t>
     </r>
@@ -1165,6 +1200,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">信息</t>
     </r>
@@ -1184,6 +1220,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">项目入职表格</t>
     </r>
@@ -1194,6 +1231,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">用于 </t>
     </r>
@@ -1211,6 +1249,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">项目入职的表格</t>
     </r>
@@ -1230,6 +1269,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">项目</t>
     </r>
@@ -1247,6 +1287,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">项目名 </t>
     </r>
@@ -1275,6 +1316,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">项目</t>
     </r>
@@ -1292,6 +1334,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">选择司法管辖区 </t>
     </r>
@@ -1311,6 +1354,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">主要赞助商</t>
     </r>
@@ -1328,6 +1372,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">法人实体 </t>
     </r>
@@ -1347,6 +1392,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">主要赞助商</t>
     </r>
@@ -1364,6 +1410,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">选择法人机构识别编码类型 </t>
     </r>
@@ -1392,6 +1439,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">法律实体标识符 </t>
     </r>
@@ -1409,6 +1457,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">全球位置编号 </t>
     </r>
@@ -1426,6 +1475,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">数据通用编号系统 </t>
     </r>
@@ -1443,6 +1493,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">公司注册号码</t>
     </r>
@@ -1453,6 +1504,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">主要赞助商</t>
     </r>
@@ -1470,6 +1522,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">法人机构编号</t>
     </r>
@@ -1487,6 +1540,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">编号 </t>
     </r>
@@ -1506,6 +1560,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">主要赞助商</t>
     </r>
@@ -1523,6 +1578,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">选择注册国家 </t>
     </r>
@@ -1542,6 +1598,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">主要联系人</t>
     </r>
@@ -1559,6 +1616,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">名字 </t>
     </r>
@@ -1578,6 +1636,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">主要联系人</t>
     </r>
@@ -1595,6 +1654,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">姓 </t>
     </r>
@@ -1614,6 +1674,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">主要联系人</t>
     </r>
@@ -1631,6 +1692,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">电邮位置 </t>
     </r>
@@ -1659,6 +1721,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">节目类型</t>
     </r>
@@ -1676,6 +1739,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">选择程序类型 </t>
     </r>
@@ -1706,6 +1770,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">社会和人道主义应用</t>
     </r>
@@ -1725,6 +1790,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">供应链</t>
     </r>
@@ -1744,6 +1810,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">协调</t>
     </r>
@@ -1763,6 +1830,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">捕获段</t>
     </r>
@@ -1773,6 +1841,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">用于实现主要可持续发展目标 </t>
     </r>
@@ -1790,6 +1859,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">的细分市场扩展</t>
     </r>
@@ -1800,6 +1870,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">操作</t>
     </r>
@@ -1817,6 +1888,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">链接的表单 </t>
     </r>
@@ -1836,6 +1908,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">可持续发展目标 </t>
     </r>
@@ -1853,6 +1926,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">主要目标</t>
     </r>
@@ -1870,6 +1944,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">选择目标 </t>
     </r>
@@ -1889,6 +1964,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">可持续发展目标 </t>
     </r>
@@ -1906,6 +1982,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">主要目标</t>
     </r>
@@ -1923,6 +2000,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">选择目标 </t>
     </r>
@@ -1951,6 +2029,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">捕获段</t>
     </r>
@@ -1961,6 +2040,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">使用全球行业分类标准 </t>
     </r>
@@ -1978,6 +2058,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">获取主要业务活动的细分市场扩展</t>
     </r>
@@ -1988,6 +2069,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">全球行业分类标准 </t>
     </r>
@@ -2005,6 +2087,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">主要业务活动</t>
     </r>
@@ -2022,6 +2105,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">选择部门 </t>
     </r>
@@ -2050,6 +2134,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">捕获段</t>
     </r>
@@ -2060,6 +2145,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">全球行业分类标准 </t>
     </r>
@@ -2077,6 +2163,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">主要业务活动</t>
     </r>
@@ -2094,6 +2181,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">选择行业组 </t>
     </r>
@@ -2113,6 +2201,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">全球行业分类标准 </t>
     </r>
@@ -2130,6 +2219,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">主要业务活动</t>
     </r>
@@ -2147,6 +2237,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">选择行业 </t>
     </r>
@@ -2166,6 +2257,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">全球行业分类标准 </t>
     </r>
@@ -2183,6 +2275,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">主要业务活动</t>
     </r>
@@ -2200,6 +2293,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">选择子行业 </t>
     </r>
@@ -2223,7 +2317,7 @@
     <numFmt numFmtId="165" formatCode="[$-F800]DDDD&quot;, &quot;MMMM\ DD&quot;, &quot;YYYY"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="28">
     <font>
       <sz val="10"/>
       <name val="Helvetica Neue"/>
@@ -2244,20 +2338,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2397,6 +2477,11 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
@@ -2414,17 +2499,20 @@
       <sz val="10"/>
       <name val="Noto Sans CJK SC"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Noto Sans CJK SC"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Noto Sans CJK SC"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="12">
@@ -2495,7 +2583,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="63">
+  <borders count="56">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -2608,51 +2696,7 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin">
-        <color rgb="FFA7A7A7"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right style="thin"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
@@ -2765,6 +2809,60 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FFDCDCDC"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFDCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFDCDCDC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFDCDCDC"/>
+      </top>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FFDCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="FFDCDCDC"/>
+      </top>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="thin">
         <color rgb="FFDCDCDC"/>
@@ -2772,6 +2870,13 @@
       <top style="thin">
         <color rgb="FFDCDCDC"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -2826,11 +2931,25 @@
       <left style="thin">
         <color rgb="FFDCDCDC"/>
       </left>
-      <right style="thin"/>
+      <right/>
       <top style="thin">
         <color rgb="FFDCDCDC"/>
       </top>
       <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -2885,81 +3004,13 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+      <left style="thin">
+        <color rgb="FFDCDCDC"/>
+      </left>
       <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin">
-        <color rgb="FFA7A7A7"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
+      <top style="thin">
+        <color rgb="FFDCDCDC"/>
+      </top>
       <bottom style="thin"/>
       <diagonal/>
     </border>
@@ -3058,7 +3109,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="24">
+  <cellStyleXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3082,613 +3133,624 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+  </cellStyleXfs>
+  <cellXfs count="150">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="145">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="23" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="3" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="5" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="5" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="5" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="6" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="7" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="8" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="8" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="9" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="5" borderId="8" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="5" borderId="8" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="5" borderId="9" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="23" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="23" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="23" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="2" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="3" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="8" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="4" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="9" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="5" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="7" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="7" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="7" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="7" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="8" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="7" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="7" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="7" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="21" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="5" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="4" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="23" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="5" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="2" borderId="5" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="6" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="7" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="8" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="23" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="8" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="9" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="8" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="10" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="10" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="40" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="41" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="42" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="43" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="44" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="45" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="46" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="47" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="7" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="7" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="7" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="8" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="9" borderId="48" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="10" borderId="49" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="50" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="9" borderId="46" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="10" borderId="51" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="10" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="8" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="9" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="6" borderId="8" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="10" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="9" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="11" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="5" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="6" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="7" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="7" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="7" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="7" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="8" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="7" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="7" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="7" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="7" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="7" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="7" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="7" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="9" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="10" borderId="53" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="54" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="47" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="55" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="47" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="11" borderId="48" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="11" borderId="46" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="11" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="25" fillId="7" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="25" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="25" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="25" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="10" borderId="49" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="26" fillId="10" borderId="51" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="10" borderId="53" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="23" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="24" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="24" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="40" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="41" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="42" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="43" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="7" borderId="44" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="7" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="7" borderId="45" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="7" borderId="46" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="7" borderId="47" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="7" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="8" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="7" borderId="48" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="7" borderId="49" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="7" borderId="50" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="7" borderId="51" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="7" borderId="51" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="7" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="7" borderId="53" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="7" borderId="54" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="9" borderId="55" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="10" borderId="56" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="9" borderId="43" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="10" borderId="58" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="59" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="59" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="59" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="9" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="10" borderId="60" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="61" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="62" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="11" borderId="55" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="11" borderId="43" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="11" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="7" borderId="45" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="7" borderId="46" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="7" borderId="48" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="7" borderId="49" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="27" fillId="10" borderId="56" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="27" fillId="10" borderId="58" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="27" fillId="10" borderId="60" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Hyperlink 2" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal 3" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="21" builtinId="53" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <dxfs count="54">
@@ -4307,9 +4369,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>123840</xdr:colOff>
+      <xdr:colOff>123480</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>91080</xdr:rowOff>
+      <xdr:rowOff>90720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4322,8 +4384,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4059720" y="281880"/>
-          <a:ext cx="2904840" cy="825120"/>
+          <a:off x="4060440" y="281880"/>
+          <a:ext cx="2904480" cy="824760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5979,10 +6041,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5994,7 +6056,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="10.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="28.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="10.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6004,351 +6068,405 @@
       <c r="D1" s="51"/>
       <c r="E1" s="51"/>
       <c r="F1" s="52"/>
-      <c r="G1" s="53"/>
+      <c r="G1" s="51"/>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="54"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="57"/>
-    </row>
-    <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="58" t="s">
+      <c r="A2" s="53"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="54"/>
+    </row>
+    <row r="3" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="59" t="s">
+      <c r="E3" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="61" t="s">
+      <c r="F3" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="60" t="s">
+      <c r="G3" s="56" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="62"/>
-      <c r="B4" s="63" t="s">
+      <c r="H3" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="C4" s="64" t="s">
+      <c r="I3" s="56" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="59"/>
+      <c r="B4" s="60" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="65"/>
-      <c r="E4" s="64" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" s="66"/>
-      <c r="G4" s="65"/>
-    </row>
-    <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="67"/>
-      <c r="B5" s="68" t="s">
-        <v>94</v>
-      </c>
-      <c r="C5" s="69" t="s">
+      <c r="D4" s="62"/>
+      <c r="E4" s="61" t="s">
+        <v>95</v>
+      </c>
+      <c r="F4" s="63"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="62"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="65"/>
+      <c r="B5" s="66" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="70"/>
-      <c r="E5" s="69" t="s">
-        <v>93</v>
-      </c>
-      <c r="F5" s="71" t="s">
+      <c r="D5" s="68"/>
+      <c r="E5" s="67" t="s">
         <v>95</v>
       </c>
-      <c r="G5" s="72" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="67"/>
-      <c r="B6" s="68" t="s">
+      <c r="F5" s="69" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="69" t="s">
+      <c r="G5" s="70" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" s="69"/>
+      <c r="I5" s="71"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="65"/>
+      <c r="B6" s="66" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="73"/>
-      <c r="E6" s="69" t="s">
-        <v>93</v>
-      </c>
-      <c r="F6" s="71"/>
-      <c r="G6" s="74"/>
-    </row>
-    <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="67"/>
-      <c r="B7" s="68" t="s">
-        <v>98</v>
-      </c>
-      <c r="C7" s="69" t="s">
+      <c r="D6" s="72"/>
+      <c r="E6" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" s="69"/>
+      <c r="G6" s="73"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="74"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="65"/>
+      <c r="B7" s="66" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="73"/>
-      <c r="E7" s="69" t="s">
-        <v>93</v>
-      </c>
-      <c r="F7" s="71"/>
-      <c r="G7" s="73" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="67"/>
-      <c r="B8" s="68" t="s">
-        <v>100</v>
+      <c r="D7" s="72"/>
+      <c r="E7" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" s="69"/>
+      <c r="G7" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="H7" s="69"/>
+      <c r="I7" s="72"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="65"/>
+      <c r="B8" s="66" t="s">
+        <v>102</v>
       </c>
       <c r="C8" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="73"/>
-      <c r="E8" s="69" t="s">
-        <v>93</v>
-      </c>
-      <c r="F8" s="71"/>
-      <c r="G8" s="73"/>
-    </row>
-    <row r="9" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="67"/>
-      <c r="B9" s="68" t="s">
-        <v>101</v>
+      <c r="D8" s="72"/>
+      <c r="E8" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" s="69"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="69"/>
+      <c r="I8" s="72"/>
+    </row>
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="65"/>
+      <c r="B9" s="66" t="s">
+        <v>103</v>
       </c>
       <c r="C9" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="73"/>
-      <c r="E9" s="69" t="s">
-        <v>93</v>
-      </c>
-      <c r="F9" s="71" t="s">
+      <c r="D9" s="72"/>
+      <c r="E9" s="67" t="s">
         <v>95</v>
       </c>
+      <c r="F9" s="69" t="s">
+        <v>97</v>
+      </c>
       <c r="G9" s="76" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="67"/>
-      <c r="B10" s="68" t="s">
-        <v>102</v>
+        <v>98</v>
+      </c>
+      <c r="H9" s="69"/>
+      <c r="I9" s="77"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="65"/>
+      <c r="B10" s="66" t="s">
+        <v>104</v>
       </c>
       <c r="C10" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="73" t="s">
-        <v>103</v>
-      </c>
-      <c r="E10" s="69" t="s">
-        <v>93</v>
-      </c>
-      <c r="F10" s="71"/>
-      <c r="G10" s="73"/>
-    </row>
-    <row r="11" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="67"/>
-      <c r="B11" s="68" t="s">
-        <v>104</v>
-      </c>
-      <c r="C11" s="69" t="s">
+      <c r="D10" s="72" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="F10" s="69"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="72"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="65"/>
+      <c r="B11" s="66" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="73" t="s">
-        <v>103</v>
-      </c>
-      <c r="E11" s="69" t="s">
-        <v>93</v>
-      </c>
-      <c r="F11" s="71"/>
-      <c r="G11" s="73"/>
-    </row>
-    <row r="12" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="67"/>
-      <c r="B12" s="68" t="s">
+      <c r="D11" s="72" t="s">
         <v>105</v>
       </c>
-      <c r="C12" s="69" t="s">
+      <c r="E11" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="69"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="69"/>
+      <c r="I11" s="72"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="65"/>
+      <c r="B12" s="66" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="73" t="s">
-        <v>103</v>
-      </c>
-      <c r="E12" s="69" t="s">
-        <v>93</v>
-      </c>
-      <c r="F12" s="71"/>
-      <c r="G12" s="77"/>
-    </row>
-    <row r="13" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="67"/>
-      <c r="B13" s="68" t="s">
-        <v>106</v>
-      </c>
-      <c r="C13" s="69" t="s">
+      <c r="D12" s="72" t="s">
+        <v>105</v>
+      </c>
+      <c r="E12" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" s="69"/>
+      <c r="G12" s="78"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="79"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="65"/>
+      <c r="B13" s="66" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="73"/>
-      <c r="E13" s="69" t="s">
-        <v>93</v>
-      </c>
-      <c r="F13" s="71"/>
-      <c r="G13" s="73" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="78"/>
-      <c r="B14" s="63" t="s">
-        <v>108</v>
-      </c>
-      <c r="C14" s="64" t="s">
+      <c r="D13" s="72"/>
+      <c r="E13" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="F13" s="69"/>
+      <c r="G13" s="80" t="s">
+        <v>109</v>
+      </c>
+      <c r="H13" s="81"/>
+      <c r="I13" s="82"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="83"/>
+      <c r="B14" s="60" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="D14" s="65"/>
-      <c r="E14" s="64" t="s">
-        <v>93</v>
-      </c>
-      <c r="F14" s="66"/>
-      <c r="G14" s="79"/>
-    </row>
-    <row r="15" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="67"/>
-      <c r="B15" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="C15" s="80" t="s">
+      <c r="D14" s="62"/>
+      <c r="E14" s="61" t="s">
+        <v>95</v>
+      </c>
+      <c r="F14" s="63"/>
+      <c r="G14" s="84"/>
+      <c r="H14" s="85" t="s">
+        <v>111</v>
+      </c>
+      <c r="I14" s="86" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="65"/>
+      <c r="B15" s="66" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="70"/>
-      <c r="E15" s="69" t="s">
-        <v>93</v>
-      </c>
-      <c r="F15" s="71" t="s">
+      <c r="D15" s="68"/>
+      <c r="E15" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="F15" s="69" t="s">
+        <v>114</v>
+      </c>
+      <c r="G15" s="88" t="s">
+        <v>98</v>
+      </c>
+      <c r="H15" s="89" t="s">
+        <v>111</v>
+      </c>
+      <c r="I15" s="90" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="91"/>
+      <c r="B16" s="92" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" s="93" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="94"/>
+      <c r="E16" s="95" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="96" t="s">
+        <v>116</v>
+      </c>
+      <c r="G16" s="97" t="s">
+        <v>98</v>
+      </c>
+      <c r="H16" s="98" t="s">
+        <v>111</v>
+      </c>
+      <c r="I16" s="99" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="100"/>
+      <c r="B17" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="G15" s="81" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="82"/>
-      <c r="B16" s="83" t="s">
-        <v>111</v>
-      </c>
-      <c r="C16" s="84" t="s">
+      <c r="C17" s="101" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="102"/>
+      <c r="E17" s="101" t="s">
+        <v>95</v>
+      </c>
+      <c r="F17" s="103"/>
+      <c r="G17" s="78"/>
+      <c r="H17" s="103"/>
+      <c r="I17" s="104"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="65"/>
+      <c r="B18" s="66" t="s">
+        <v>117</v>
+      </c>
+      <c r="C18" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="85"/>
-      <c r="E16" s="86" t="s">
-        <v>93</v>
-      </c>
-      <c r="F16" s="87" t="s">
-        <v>112</v>
-      </c>
-      <c r="G16" s="88" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="89"/>
-      <c r="B17" s="63" t="s">
-        <v>108</v>
-      </c>
-      <c r="C17" s="90" t="s">
-        <v>59</v>
-      </c>
-      <c r="D17" s="91"/>
-      <c r="E17" s="90" t="s">
-        <v>93</v>
-      </c>
-      <c r="F17" s="92"/>
-      <c r="G17" s="93"/>
-    </row>
-    <row r="18" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="67"/>
-      <c r="B18" s="68" t="s">
-        <v>113</v>
-      </c>
-      <c r="C18" s="80" t="s">
+      <c r="D18" s="72"/>
+      <c r="E18" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="F18" s="69" t="s">
+        <v>118</v>
+      </c>
+      <c r="G18" s="105" t="s">
+        <v>98</v>
+      </c>
+      <c r="H18" s="69"/>
+      <c r="I18" s="106"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="65"/>
+      <c r="B19" s="107" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" s="108" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="73"/>
-      <c r="E18" s="69" t="s">
-        <v>93</v>
-      </c>
-      <c r="F18" s="71" t="s">
-        <v>114</v>
-      </c>
-      <c r="G18" s="94" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="67"/>
-      <c r="B19" s="95" t="s">
-        <v>115</v>
-      </c>
-      <c r="C19" s="96" t="s">
+      <c r="D19" s="109"/>
+      <c r="E19" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="F19" s="69" t="s">
+        <v>120</v>
+      </c>
+      <c r="G19" s="105" t="s">
+        <v>98</v>
+      </c>
+      <c r="H19" s="69"/>
+      <c r="I19" s="106"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="65"/>
+      <c r="B20" s="107" t="s">
+        <v>121</v>
+      </c>
+      <c r="C20" s="108" t="s">
         <v>53</v>
       </c>
-      <c r="D19" s="97"/>
-      <c r="E19" s="69" t="s">
-        <v>93</v>
-      </c>
-      <c r="F19" s="71" t="s">
-        <v>116</v>
-      </c>
-      <c r="G19" s="94" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="67"/>
-      <c r="B20" s="95" t="s">
-        <v>117</v>
-      </c>
-      <c r="C20" s="96" t="s">
+      <c r="D20" s="109"/>
+      <c r="E20" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="F20" s="69" t="s">
+        <v>122</v>
+      </c>
+      <c r="G20" s="105" t="s">
+        <v>98</v>
+      </c>
+      <c r="H20" s="69"/>
+      <c r="I20" s="106"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="91"/>
+      <c r="B21" s="92" t="s">
+        <v>123</v>
+      </c>
+      <c r="C21" s="93" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="97"/>
-      <c r="E20" s="69" t="s">
-        <v>93</v>
-      </c>
-      <c r="F20" s="71" t="s">
-        <v>118</v>
-      </c>
-      <c r="G20" s="94" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="82"/>
-      <c r="B21" s="83" t="s">
-        <v>119</v>
-      </c>
-      <c r="C21" s="84" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21" s="98"/>
-      <c r="E21" s="86" t="s">
-        <v>93</v>
-      </c>
-      <c r="F21" s="87" t="s">
-        <v>120</v>
-      </c>
-      <c r="G21" s="99" t="s">
-        <v>96</v>
-      </c>
+      <c r="D21" s="110"/>
+      <c r="E21" s="95" t="s">
+        <v>95</v>
+      </c>
+      <c r="F21" s="96" t="s">
+        <v>124</v>
+      </c>
+      <c r="G21" s="111" t="s">
+        <v>98</v>
+      </c>
+      <c r="H21" s="96"/>
+      <c r="I21" s="112"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -6368,7 +6486,7 @@
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -6384,340 +6502,340 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="100"/>
-      <c r="B1" s="101"/>
+      <c r="A1" s="113"/>
+      <c r="B1" s="114"/>
       <c r="C1" s="51"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="102" t="s">
+      <c r="D1" s="51"/>
+      <c r="E1" s="56" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" s="57" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="115"/>
+      <c r="B2" s="115"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="117" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" s="118" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="119" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="119" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" s="117" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="117" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="57" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="120" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="121" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="60" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="62" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" s="122"/>
+      <c r="F4" s="62"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="123" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="124" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="66" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="72" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="125"/>
+      <c r="F5" s="72"/>
+    </row>
+    <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="123" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" s="124" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="66" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="72" t="s">
+        <v>133</v>
+      </c>
+      <c r="E6" s="125"/>
+      <c r="F6" s="72"/>
+    </row>
+    <row r="7" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="123" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="124" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" s="66" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="E7" s="125" t="s">
+        <v>135</v>
+      </c>
+      <c r="F7" s="72"/>
+    </row>
+    <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="123" t="s">
+        <v>129</v>
+      </c>
+      <c r="B8" s="124" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" s="66" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="72" t="s">
+        <v>136</v>
+      </c>
+      <c r="E8" s="126"/>
+      <c r="F8" s="74"/>
+    </row>
+    <row r="9" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="123" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" s="124" t="s">
+        <v>130</v>
+      </c>
+      <c r="C9" s="66" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="72" t="s">
+        <v>137</v>
+      </c>
+      <c r="E9" s="126"/>
+      <c r="F9" s="74"/>
+    </row>
+    <row r="10" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="123" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" s="124" t="s">
+        <v>130</v>
+      </c>
+      <c r="C10" s="66" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="72" t="s">
+        <v>138</v>
+      </c>
+      <c r="E10" s="127"/>
+      <c r="F10" s="72"/>
+    </row>
+    <row r="11" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="123" t="s">
+        <v>129</v>
+      </c>
+      <c r="B11" s="124" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" s="66" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" s="72" t="s">
+        <v>139</v>
+      </c>
+      <c r="E11" s="127"/>
+      <c r="F11" s="72"/>
+    </row>
+    <row r="12" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="123" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" s="124" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" s="66" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" s="72" t="s">
+        <v>140</v>
+      </c>
+      <c r="E12" s="127"/>
+      <c r="F12" s="72"/>
+    </row>
+    <row r="13" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="128" t="s">
+        <v>129</v>
+      </c>
+      <c r="B13" s="129" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" s="130" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" s="131" t="s">
+        <v>141</v>
+      </c>
+      <c r="E13" s="132" t="s">
+        <v>142</v>
+      </c>
+      <c r="F13" s="133"/>
+    </row>
+    <row r="14" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="134" t="s">
+        <v>143</v>
+      </c>
+      <c r="B14" s="121" t="s">
+        <v>144</v>
+      </c>
+      <c r="C14" s="120" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="60" t="s">
+        <v>145</v>
+      </c>
+      <c r="E14" s="122"/>
+      <c r="F14" s="62"/>
+    </row>
+    <row r="15" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="135" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15" s="124" t="s">
+        <v>144</v>
+      </c>
+      <c r="C15" s="66" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" s="72" t="s">
+        <v>146</v>
+      </c>
+      <c r="E15" s="127"/>
+      <c r="F15" s="136"/>
+    </row>
+    <row r="16" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="137" t="s">
+        <v>143</v>
+      </c>
+      <c r="B16" s="129" t="s">
+        <v>144</v>
+      </c>
+      <c r="C16" s="92" t="s">
+        <v>115</v>
+      </c>
+      <c r="D16" s="138" t="s">
+        <v>147</v>
+      </c>
+      <c r="E16" s="132"/>
+      <c r="F16" s="133"/>
+    </row>
+    <row r="17" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="134" t="s">
+        <v>148</v>
+      </c>
+      <c r="B17" s="121" t="s">
+        <v>149</v>
+      </c>
+      <c r="C17" s="120" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="60" t="s">
+        <v>145</v>
+      </c>
+      <c r="E17" s="122"/>
+      <c r="F17" s="62"/>
+    </row>
+    <row r="18" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="135" t="s">
+        <v>148</v>
+      </c>
+      <c r="B18" s="124" t="s">
+        <v>149</v>
+      </c>
+      <c r="C18" s="66" t="s">
+        <v>117</v>
+      </c>
+      <c r="D18" s="72" t="s">
+        <v>150</v>
+      </c>
+      <c r="E18" s="127"/>
+      <c r="F18" s="136"/>
+    </row>
+    <row r="19" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="135" t="s">
+        <v>148</v>
+      </c>
+      <c r="B19" s="124" t="s">
+        <v>149</v>
+      </c>
+      <c r="C19" s="107" t="s">
+        <v>119</v>
+      </c>
+      <c r="D19" s="66" t="s">
+        <v>151</v>
+      </c>
+      <c r="E19" s="127"/>
+      <c r="F19" s="136"/>
+    </row>
+    <row r="20" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="135" t="s">
+        <v>148</v>
+      </c>
+      <c r="B20" s="124" t="s">
+        <v>149</v>
+      </c>
+      <c r="C20" s="107" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="103" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="104"/>
-      <c r="B2" s="105"/>
-      <c r="C2" s="106"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="107" t="s">
-        <v>122</v>
-      </c>
-      <c r="F2" s="108" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="109" t="s">
+      <c r="D20" s="66" t="s">
+        <v>152</v>
+      </c>
+      <c r="E20" s="127"/>
+      <c r="F20" s="72"/>
+    </row>
+    <row r="21" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="137" t="s">
+        <v>148</v>
+      </c>
+      <c r="B21" s="129" t="s">
+        <v>149</v>
+      </c>
+      <c r="C21" s="92" t="s">
         <v>123</v>
       </c>
-      <c r="B3" s="110" t="s">
-        <v>124</v>
-      </c>
-      <c r="C3" s="111" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="112" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="113" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" s="114" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="115" t="s">
-        <v>125</v>
-      </c>
-      <c r="B4" s="116" t="s">
-        <v>126</v>
-      </c>
-      <c r="C4" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" s="65" t="s">
-        <v>127</v>
-      </c>
-      <c r="E4" s="117"/>
-      <c r="F4" s="65"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="118" t="s">
-        <v>125</v>
-      </c>
-      <c r="B5" s="119" t="s">
-        <v>126</v>
-      </c>
-      <c r="C5" s="68" t="s">
-        <v>94</v>
-      </c>
-      <c r="D5" s="73" t="s">
-        <v>128</v>
-      </c>
-      <c r="E5" s="120"/>
-      <c r="F5" s="73"/>
-    </row>
-    <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="118" t="s">
-        <v>125</v>
-      </c>
-      <c r="B6" s="119" t="s">
-        <v>126</v>
-      </c>
-      <c r="C6" s="68" t="s">
-        <v>97</v>
-      </c>
-      <c r="D6" s="73" t="s">
-        <v>129</v>
-      </c>
-      <c r="E6" s="120"/>
-      <c r="F6" s="73"/>
-    </row>
-    <row r="7" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="118" t="s">
-        <v>125</v>
-      </c>
-      <c r="B7" s="119" t="s">
-        <v>126</v>
-      </c>
-      <c r="C7" s="68" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" s="73" t="s">
-        <v>130</v>
-      </c>
-      <c r="E7" s="120" t="s">
-        <v>131</v>
-      </c>
-      <c r="F7" s="73"/>
-    </row>
-    <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="118" t="s">
-        <v>125</v>
-      </c>
-      <c r="B8" s="119" t="s">
-        <v>126</v>
-      </c>
-      <c r="C8" s="68" t="s">
-        <v>100</v>
-      </c>
-      <c r="D8" s="73" t="s">
-        <v>132</v>
-      </c>
-      <c r="E8" s="121"/>
-      <c r="F8" s="74"/>
-    </row>
-    <row r="9" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="118" t="s">
-        <v>125</v>
-      </c>
-      <c r="B9" s="119" t="s">
-        <v>126</v>
-      </c>
-      <c r="C9" s="68" t="s">
-        <v>101</v>
-      </c>
-      <c r="D9" s="73" t="s">
-        <v>133</v>
-      </c>
-      <c r="E9" s="121"/>
-      <c r="F9" s="74"/>
-    </row>
-    <row r="10" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="118" t="s">
-        <v>125</v>
-      </c>
-      <c r="B10" s="119" t="s">
-        <v>126</v>
-      </c>
-      <c r="C10" s="68" t="s">
-        <v>102</v>
-      </c>
-      <c r="D10" s="73" t="s">
-        <v>134</v>
-      </c>
-      <c r="E10" s="122"/>
-      <c r="F10" s="73"/>
-    </row>
-    <row r="11" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="118" t="s">
-        <v>125</v>
-      </c>
-      <c r="B11" s="119" t="s">
-        <v>126</v>
-      </c>
-      <c r="C11" s="68" t="s">
-        <v>104</v>
-      </c>
-      <c r="D11" s="73" t="s">
-        <v>135</v>
-      </c>
-      <c r="E11" s="122"/>
-      <c r="F11" s="73"/>
-    </row>
-    <row r="12" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="118" t="s">
-        <v>125</v>
-      </c>
-      <c r="B12" s="119" t="s">
-        <v>126</v>
-      </c>
-      <c r="C12" s="68" t="s">
-        <v>105</v>
-      </c>
-      <c r="D12" s="73" t="s">
-        <v>136</v>
-      </c>
-      <c r="E12" s="122"/>
-      <c r="F12" s="73"/>
-    </row>
-    <row r="13" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="123" t="s">
-        <v>125</v>
-      </c>
-      <c r="B13" s="124" t="s">
-        <v>126</v>
-      </c>
-      <c r="C13" s="125" t="s">
-        <v>106</v>
-      </c>
-      <c r="D13" s="126" t="s">
-        <v>137</v>
-      </c>
-      <c r="E13" s="127" t="s">
-        <v>138</v>
-      </c>
-      <c r="F13" s="128"/>
-    </row>
-    <row r="14" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="129" t="s">
-        <v>139</v>
-      </c>
-      <c r="B14" s="116" t="s">
-        <v>140</v>
-      </c>
-      <c r="C14" s="115" t="s">
-        <v>108</v>
-      </c>
-      <c r="D14" s="63" t="s">
-        <v>141</v>
-      </c>
-      <c r="E14" s="117"/>
-      <c r="F14" s="65"/>
-    </row>
-    <row r="15" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="130" t="s">
-        <v>139</v>
-      </c>
-      <c r="B15" s="119" t="s">
-        <v>140</v>
-      </c>
-      <c r="C15" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="D15" s="73" t="s">
-        <v>142</v>
-      </c>
-      <c r="E15" s="122"/>
-      <c r="F15" s="131"/>
-    </row>
-    <row r="16" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="132" t="s">
-        <v>139</v>
-      </c>
-      <c r="B16" s="124" t="s">
-        <v>140</v>
-      </c>
-      <c r="C16" s="83" t="s">
-        <v>111</v>
-      </c>
-      <c r="D16" s="133" t="s">
-        <v>143</v>
-      </c>
-      <c r="E16" s="127"/>
-      <c r="F16" s="128"/>
-    </row>
-    <row r="17" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="129" t="s">
-        <v>144</v>
-      </c>
-      <c r="B17" s="116" t="s">
-        <v>145</v>
-      </c>
-      <c r="C17" s="115" t="s">
-        <v>108</v>
-      </c>
-      <c r="D17" s="63" t="s">
-        <v>141</v>
-      </c>
-      <c r="E17" s="117"/>
-      <c r="F17" s="65"/>
-    </row>
-    <row r="18" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="130" t="s">
-        <v>144</v>
-      </c>
-      <c r="B18" s="119" t="s">
-        <v>145</v>
-      </c>
-      <c r="C18" s="68" t="s">
-        <v>113</v>
-      </c>
-      <c r="D18" s="73" t="s">
-        <v>146</v>
-      </c>
-      <c r="E18" s="122"/>
-      <c r="F18" s="131"/>
-    </row>
-    <row r="19" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="130" t="s">
-        <v>144</v>
-      </c>
-      <c r="B19" s="119" t="s">
-        <v>145</v>
-      </c>
-      <c r="C19" s="95" t="s">
-        <v>115</v>
-      </c>
-      <c r="D19" s="68" t="s">
-        <v>147</v>
-      </c>
-      <c r="E19" s="122"/>
-      <c r="F19" s="131"/>
-    </row>
-    <row r="20" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="130" t="s">
-        <v>144</v>
-      </c>
-      <c r="B20" s="119" t="s">
-        <v>145</v>
-      </c>
-      <c r="C20" s="95" t="s">
-        <v>117</v>
-      </c>
-      <c r="D20" s="68" t="s">
-        <v>148</v>
-      </c>
-      <c r="E20" s="122"/>
-      <c r="F20" s="73"/>
-    </row>
-    <row r="21" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="132" t="s">
-        <v>144</v>
-      </c>
-      <c r="B21" s="124" t="s">
-        <v>145</v>
-      </c>
-      <c r="C21" s="83" t="s">
-        <v>119</v>
-      </c>
-      <c r="D21" s="133" t="s">
-        <v>149</v>
-      </c>
-      <c r="E21" s="127"/>
-      <c r="F21" s="128"/>
+      <c r="D21" s="138" t="s">
+        <v>153</v>
+      </c>
+      <c r="E21" s="132"/>
+      <c r="F21" s="133"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -6753,340 +6871,340 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="100"/>
-      <c r="B1" s="101"/>
+      <c r="A1" s="113"/>
+      <c r="B1" s="114"/>
       <c r="C1" s="51"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="134" t="s">
-        <v>150</v>
-      </c>
-      <c r="F1" s="135" t="s">
-        <v>150</v>
+      <c r="D1" s="51"/>
+      <c r="E1" s="139" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" s="140" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="104"/>
-      <c r="B2" s="105"/>
-      <c r="C2" s="106"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="136" t="s">
-        <v>151</v>
-      </c>
-      <c r="F2" s="137" t="s">
-        <v>151</v>
+      <c r="A2" s="115"/>
+      <c r="B2" s="115"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="141" t="s">
+        <v>155</v>
+      </c>
+      <c r="F2" s="142" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="109" t="s">
-        <v>152</v>
-      </c>
-      <c r="B3" s="110" t="s">
-        <v>153</v>
-      </c>
-      <c r="C3" s="111" t="s">
-        <v>154</v>
-      </c>
-      <c r="D3" s="112" t="s">
-        <v>155</v>
-      </c>
-      <c r="E3" s="113" t="s">
+      <c r="A3" s="119" t="s">
         <v>156</v>
       </c>
-      <c r="F3" s="114" t="s">
+      <c r="B3" s="119" t="s">
         <v>157</v>
       </c>
+      <c r="C3" s="117" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3" s="117" t="s">
+        <v>159</v>
+      </c>
+      <c r="E3" s="56" t="s">
+        <v>160</v>
+      </c>
+      <c r="F3" s="57" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="115" t="s">
-        <v>158</v>
-      </c>
-      <c r="B4" s="138" t="s">
-        <v>159</v>
-      </c>
-      <c r="C4" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" s="65" t="s">
-        <v>160</v>
-      </c>
-      <c r="E4" s="117"/>
-      <c r="F4" s="65"/>
+      <c r="A4" s="120" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4" s="143" t="s">
+        <v>163</v>
+      </c>
+      <c r="C4" s="60" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="62" t="s">
+        <v>164</v>
+      </c>
+      <c r="E4" s="122"/>
+      <c r="F4" s="62"/>
     </row>
     <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="118" t="s">
-        <v>158</v>
-      </c>
-      <c r="B5" s="139" t="s">
-        <v>159</v>
-      </c>
-      <c r="C5" s="68" t="s">
-        <v>94</v>
-      </c>
-      <c r="D5" s="73" t="s">
-        <v>161</v>
-      </c>
-      <c r="E5" s="120"/>
-      <c r="F5" s="73"/>
+      <c r="A5" s="123" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="144" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="66" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="72" t="s">
+        <v>165</v>
+      </c>
+      <c r="E5" s="125"/>
+      <c r="F5" s="72"/>
     </row>
     <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="118" t="s">
-        <v>158</v>
-      </c>
-      <c r="B6" s="139" t="s">
-        <v>159</v>
-      </c>
-      <c r="C6" s="68" t="s">
-        <v>97</v>
-      </c>
-      <c r="D6" s="140" t="s">
+      <c r="A6" s="123" t="s">
         <v>162</v>
       </c>
-      <c r="E6" s="120"/>
-      <c r="F6" s="73"/>
+      <c r="B6" s="144" t="s">
+        <v>163</v>
+      </c>
+      <c r="C6" s="66" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="145" t="s">
+        <v>166</v>
+      </c>
+      <c r="E6" s="125"/>
+      <c r="F6" s="72"/>
     </row>
     <row r="7" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="118" t="s">
-        <v>158</v>
-      </c>
-      <c r="B7" s="139" t="s">
-        <v>159</v>
-      </c>
-      <c r="C7" s="68" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" s="140" t="s">
+      <c r="A7" s="123" t="s">
+        <v>162</v>
+      </c>
+      <c r="B7" s="144" t="s">
         <v>163</v>
       </c>
-      <c r="E7" s="120" t="s">
-        <v>164</v>
-      </c>
-      <c r="F7" s="73"/>
+      <c r="C7" s="66" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="145" t="s">
+        <v>167</v>
+      </c>
+      <c r="E7" s="125" t="s">
+        <v>168</v>
+      </c>
+      <c r="F7" s="72"/>
     </row>
     <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="118" t="s">
-        <v>158</v>
-      </c>
-      <c r="B8" s="139" t="s">
-        <v>159</v>
-      </c>
-      <c r="C8" s="68" t="s">
-        <v>100</v>
-      </c>
-      <c r="D8" s="140" t="s">
-        <v>165</v>
-      </c>
-      <c r="E8" s="121"/>
+      <c r="A8" s="123" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8" s="144" t="s">
+        <v>163</v>
+      </c>
+      <c r="C8" s="66" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="145" t="s">
+        <v>169</v>
+      </c>
+      <c r="E8" s="126"/>
       <c r="F8" s="74"/>
     </row>
     <row r="9" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="118" t="s">
-        <v>158</v>
-      </c>
-      <c r="B9" s="139" t="s">
-        <v>159</v>
-      </c>
-      <c r="C9" s="68" t="s">
-        <v>101</v>
-      </c>
-      <c r="D9" s="140" t="s">
-        <v>166</v>
-      </c>
-      <c r="E9" s="121"/>
+      <c r="A9" s="123" t="s">
+        <v>162</v>
+      </c>
+      <c r="B9" s="144" t="s">
+        <v>163</v>
+      </c>
+      <c r="C9" s="66" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="145" t="s">
+        <v>170</v>
+      </c>
+      <c r="E9" s="126"/>
       <c r="F9" s="74"/>
     </row>
     <row r="10" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="118" t="s">
-        <v>158</v>
-      </c>
-      <c r="B10" s="139" t="s">
-        <v>159</v>
-      </c>
-      <c r="C10" s="68" t="s">
-        <v>102</v>
-      </c>
-      <c r="D10" s="140" t="s">
-        <v>167</v>
-      </c>
-      <c r="E10" s="122"/>
-      <c r="F10" s="73"/>
+      <c r="A10" s="123" t="s">
+        <v>162</v>
+      </c>
+      <c r="B10" s="144" t="s">
+        <v>163</v>
+      </c>
+      <c r="C10" s="66" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="145" t="s">
+        <v>171</v>
+      </c>
+      <c r="E10" s="127"/>
+      <c r="F10" s="72"/>
     </row>
     <row r="11" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="118" t="s">
-        <v>158</v>
-      </c>
-      <c r="B11" s="139" t="s">
-        <v>159</v>
-      </c>
-      <c r="C11" s="68" t="s">
-        <v>104</v>
-      </c>
-      <c r="D11" s="140" t="s">
-        <v>168</v>
-      </c>
-      <c r="E11" s="122"/>
-      <c r="F11" s="73"/>
+      <c r="A11" s="123" t="s">
+        <v>162</v>
+      </c>
+      <c r="B11" s="144" t="s">
+        <v>163</v>
+      </c>
+      <c r="C11" s="66" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" s="145" t="s">
+        <v>172</v>
+      </c>
+      <c r="E11" s="127"/>
+      <c r="F11" s="72"/>
     </row>
     <row r="12" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="118" t="s">
-        <v>158</v>
-      </c>
-      <c r="B12" s="139" t="s">
-        <v>159</v>
-      </c>
-      <c r="C12" s="68" t="s">
-        <v>105</v>
-      </c>
-      <c r="D12" s="140" t="s">
-        <v>169</v>
-      </c>
-      <c r="E12" s="122"/>
-      <c r="F12" s="73"/>
+      <c r="A12" s="123" t="s">
+        <v>162</v>
+      </c>
+      <c r="B12" s="144" t="s">
+        <v>163</v>
+      </c>
+      <c r="C12" s="66" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" s="145" t="s">
+        <v>173</v>
+      </c>
+      <c r="E12" s="127"/>
+      <c r="F12" s="72"/>
     </row>
     <row r="13" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="123" t="s">
-        <v>158</v>
-      </c>
-      <c r="B13" s="141" t="s">
-        <v>159</v>
-      </c>
-      <c r="C13" s="125" t="s">
-        <v>106</v>
-      </c>
-      <c r="D13" s="126" t="s">
-        <v>170</v>
-      </c>
-      <c r="E13" s="127" t="s">
-        <v>171</v>
-      </c>
-      <c r="F13" s="128"/>
+      <c r="A13" s="128" t="s">
+        <v>162</v>
+      </c>
+      <c r="B13" s="146" t="s">
+        <v>163</v>
+      </c>
+      <c r="C13" s="130" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" s="131" t="s">
+        <v>174</v>
+      </c>
+      <c r="E13" s="132" t="s">
+        <v>175</v>
+      </c>
+      <c r="F13" s="133"/>
     </row>
     <row r="14" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="129" t="s">
-        <v>172</v>
-      </c>
-      <c r="B14" s="138" t="s">
-        <v>173</v>
-      </c>
-      <c r="C14" s="115" t="s">
-        <v>108</v>
-      </c>
-      <c r="D14" s="142" t="s">
-        <v>174</v>
-      </c>
-      <c r="E14" s="117"/>
-      <c r="F14" s="65"/>
+      <c r="A14" s="134" t="s">
+        <v>176</v>
+      </c>
+      <c r="B14" s="143" t="s">
+        <v>177</v>
+      </c>
+      <c r="C14" s="120" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="147" t="s">
+        <v>178</v>
+      </c>
+      <c r="E14" s="122"/>
+      <c r="F14" s="62"/>
     </row>
     <row r="15" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="130" t="s">
-        <v>172</v>
-      </c>
-      <c r="B15" s="139" t="s">
-        <v>173</v>
-      </c>
-      <c r="C15" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="D15" s="140" t="s">
-        <v>175</v>
-      </c>
-      <c r="E15" s="122"/>
-      <c r="F15" s="131"/>
+      <c r="A15" s="135" t="s">
+        <v>176</v>
+      </c>
+      <c r="B15" s="144" t="s">
+        <v>177</v>
+      </c>
+      <c r="C15" s="66" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" s="145" t="s">
+        <v>179</v>
+      </c>
+      <c r="E15" s="127"/>
+      <c r="F15" s="136"/>
     </row>
     <row r="16" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="132" t="s">
-        <v>172</v>
-      </c>
-      <c r="B16" s="141" t="s">
-        <v>173</v>
-      </c>
-      <c r="C16" s="83" t="s">
-        <v>111</v>
-      </c>
-      <c r="D16" s="143" t="s">
+      <c r="A16" s="137" t="s">
         <v>176</v>
       </c>
-      <c r="E16" s="127"/>
-      <c r="F16" s="128"/>
+      <c r="B16" s="146" t="s">
+        <v>177</v>
+      </c>
+      <c r="C16" s="92" t="s">
+        <v>115</v>
+      </c>
+      <c r="D16" s="148" t="s">
+        <v>180</v>
+      </c>
+      <c r="E16" s="132"/>
+      <c r="F16" s="133"/>
     </row>
     <row r="17" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="129" t="s">
-        <v>177</v>
-      </c>
-      <c r="B17" s="138" t="s">
+      <c r="A17" s="134" t="s">
+        <v>181</v>
+      </c>
+      <c r="B17" s="143" t="s">
+        <v>182</v>
+      </c>
+      <c r="C17" s="120" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="147" t="s">
         <v>178</v>
       </c>
-      <c r="C17" s="115" t="s">
-        <v>108</v>
-      </c>
-      <c r="D17" s="142" t="s">
-        <v>174</v>
-      </c>
-      <c r="E17" s="117"/>
-      <c r="F17" s="65"/>
+      <c r="E17" s="122"/>
+      <c r="F17" s="62"/>
     </row>
     <row r="18" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="130" t="s">
-        <v>177</v>
-      </c>
-      <c r="B18" s="139" t="s">
-        <v>178</v>
-      </c>
-      <c r="C18" s="68" t="s">
-        <v>113</v>
-      </c>
-      <c r="D18" s="140" t="s">
-        <v>179</v>
-      </c>
-      <c r="E18" s="122"/>
-      <c r="F18" s="131"/>
+      <c r="A18" s="135" t="s">
+        <v>181</v>
+      </c>
+      <c r="B18" s="144" t="s">
+        <v>182</v>
+      </c>
+      <c r="C18" s="66" t="s">
+        <v>117</v>
+      </c>
+      <c r="D18" s="145" t="s">
+        <v>183</v>
+      </c>
+      <c r="E18" s="127"/>
+      <c r="F18" s="136"/>
     </row>
     <row r="19" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="130" t="s">
-        <v>180</v>
-      </c>
-      <c r="B19" s="139" t="s">
-        <v>178</v>
-      </c>
-      <c r="C19" s="95" t="s">
-        <v>115</v>
-      </c>
-      <c r="D19" s="144" t="s">
+      <c r="A19" s="135" t="s">
+        <v>184</v>
+      </c>
+      <c r="B19" s="144" t="s">
+        <v>182</v>
+      </c>
+      <c r="C19" s="107" t="s">
+        <v>119</v>
+      </c>
+      <c r="D19" s="149" t="s">
+        <v>185</v>
+      </c>
+      <c r="E19" s="127"/>
+      <c r="F19" s="136"/>
+    </row>
+    <row r="20" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="135" t="s">
         <v>181</v>
       </c>
-      <c r="E19" s="122"/>
-      <c r="F19" s="131"/>
-    </row>
-    <row r="20" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="130" t="s">
-        <v>177</v>
-      </c>
-      <c r="B20" s="139" t="s">
-        <v>178</v>
-      </c>
-      <c r="C20" s="95" t="s">
-        <v>117</v>
-      </c>
-      <c r="D20" s="144" t="s">
+      <c r="B20" s="144" t="s">
         <v>182</v>
       </c>
-      <c r="E20" s="122"/>
-      <c r="F20" s="73"/>
+      <c r="C20" s="107" t="s">
+        <v>121</v>
+      </c>
+      <c r="D20" s="149" t="s">
+        <v>186</v>
+      </c>
+      <c r="E20" s="127"/>
+      <c r="F20" s="72"/>
     </row>
     <row r="21" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="132" t="s">
-        <v>177</v>
-      </c>
-      <c r="B21" s="141" t="s">
-        <v>178</v>
-      </c>
-      <c r="C21" s="83" t="s">
-        <v>119</v>
-      </c>
-      <c r="D21" s="143" t="s">
-        <v>183</v>
-      </c>
-      <c r="E21" s="127"/>
-      <c r="F21" s="128"/>
+      <c r="A21" s="137" t="s">
+        <v>181</v>
+      </c>
+      <c r="B21" s="146" t="s">
+        <v>182</v>
+      </c>
+      <c r="C21" s="92" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" s="148" t="s">
+        <v>187</v>
+      </c>
+      <c r="E21" s="132"/>
+      <c r="F21" s="133"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Add returning errors per row in OCA XLS parser
</commit_message>
<xml_diff>
--- a/tests/assets/oca_template.xlsx
+++ b/tests/assets/oca_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="READ ME" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="188">
   <si>
     <t xml:space="preserve">OCA DATA CAPTURE SPECIFICATION</t>
   </si>
@@ -824,9 +824,6 @@
     <t xml:space="preserve">ISO 3166-2</t>
   </si>
   <si>
-    <t xml:space="preserve">[SAI]</t>
-  </si>
-  <si>
     <t xml:space="preserve">legalEntity</t>
   </si>
   <si>
@@ -863,26 +860,13 @@
     <t xml:space="preserve">linkedForm</t>
   </si>
   <si>
+    <t xml:space="preserve">SAI:linkedFormSAI</t>
+  </si>
+  <si>
     <t xml:space="preserve">${0}==‘LEI’ || ${1}==‘SHAP’</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">legalEntityType,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">programmeType</t>
-    </r>
+    <t xml:space="preserve">legalEntityType,programmeType</t>
   </si>
   <si>
     <t xml:space="preserve">SDG_goal</t>
@@ -2317,7 +2301,7 @@
     <numFmt numFmtId="165" formatCode="[$-F800]DDDD&quot;, &quot;MMMM\ DD&quot;, &quot;YYYY"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="27">
     <font>
       <sz val="10"/>
       <name val="Helvetica Neue"/>
@@ -2474,11 +2458,6 @@
       <name val="Helvetica Neue (Body)"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2843,6 +2822,17 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
+      <right style="thin">
+        <color rgb="FFDCDCDC"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFDCDCDC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
       <right/>
       <top style="thin"/>
       <bottom/>
@@ -2955,17 +2945,6 @@
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right style="thin"/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFDCDCDC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin">
-        <color rgb="FFDCDCDC"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color rgb="FFDCDCDC"/>
@@ -3141,7 +3120,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="151">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3478,19 +3457,23 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="23" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3502,24 +3485,20 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="20" fillId="0" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -3530,20 +3509,20 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="40" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="40" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="41" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="41" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="42" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="42" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="20" fillId="0" borderId="43" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -3562,19 +3541,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="46" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3582,15 +3553,23 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="47" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="40" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="47" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3630,7 +3609,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="50" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="50" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3650,11 +3629,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="9" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="52" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="9" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3670,11 +3649,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="55" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="47" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="55" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="47" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3686,59 +3665,63 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="11" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="25" fillId="7" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="25" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="25" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="25" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="10" borderId="49" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="11" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="48" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="24" fillId="7" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="24" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="24" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="24" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="25" fillId="10" borderId="49" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="26" fillId="10" borderId="51" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="25" fillId="10" borderId="51" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="10" borderId="53" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="25" fillId="10" borderId="53" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4369,9 +4352,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>123480</xdr:colOff>
+      <xdr:colOff>122400</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>90720</xdr:rowOff>
+      <xdr:rowOff>89640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4385,7 +4368,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4060440" y="281880"/>
-          <a:ext cx="2904480" cy="824760"/>
+          <a:ext cx="2903400" cy="823680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6041,10 +6024,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6057,7 +6040,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="28.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="28.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="10.59"/>
   </cols>
   <sheetData>
@@ -6140,16 +6123,14 @@
       <c r="F5" s="69" t="s">
         <v>97</v>
       </c>
-      <c r="G5" s="70" t="s">
-        <v>98</v>
-      </c>
+      <c r="G5" s="70"/>
       <c r="H5" s="69"/>
       <c r="I5" s="71"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="65"/>
       <c r="B6" s="66" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C6" s="67" t="s">
         <v>53</v>
@@ -6166,7 +6147,7 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="65"/>
       <c r="B7" s="66" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C7" s="67" t="s">
         <v>53</v>
@@ -6177,7 +6158,7 @@
       </c>
       <c r="F7" s="69"/>
       <c r="G7" s="64" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H7" s="69"/>
       <c r="I7" s="72"/>
@@ -6185,7 +6166,7 @@
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="65"/>
       <c r="B8" s="66" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C8" s="75" t="s">
         <v>53</v>
@@ -6202,7 +6183,7 @@
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="65"/>
       <c r="B9" s="66" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C9" s="75" t="s">
         <v>53</v>
@@ -6214,22 +6195,20 @@
       <c r="F9" s="69" t="s">
         <v>97</v>
       </c>
-      <c r="G9" s="76" t="s">
-        <v>98</v>
-      </c>
+      <c r="G9" s="76"/>
       <c r="H9" s="69"/>
       <c r="I9" s="77"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="65"/>
       <c r="B10" s="66" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C10" s="75" t="s">
         <v>53</v>
       </c>
       <c r="D10" s="72" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E10" s="67" t="s">
         <v>95</v>
@@ -6242,13 +6221,13 @@
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="65"/>
       <c r="B11" s="66" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C11" s="67" t="s">
         <v>53</v>
       </c>
       <c r="D11" s="72" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E11" s="67" t="s">
         <v>95</v>
@@ -6261,13 +6240,13 @@
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="65"/>
       <c r="B12" s="66" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C12" s="67" t="s">
         <v>53</v>
       </c>
       <c r="D12" s="72" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E12" s="67" t="s">
         <v>95</v>
@@ -6280,7 +6259,7 @@
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="65"/>
       <c r="B13" s="66" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C13" s="67" t="s">
         <v>53</v>
@@ -6291,7 +6270,7 @@
       </c>
       <c r="F13" s="69"/>
       <c r="G13" s="80" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H13" s="81"/>
       <c r="I13" s="82"/>
@@ -6299,21 +6278,21 @@
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="83"/>
       <c r="B14" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="84" t="s">
         <v>110</v>
-      </c>
-      <c r="C14" s="61" t="s">
-        <v>59</v>
       </c>
       <c r="D14" s="62"/>
       <c r="E14" s="61" t="s">
         <v>95</v>
       </c>
       <c r="F14" s="63"/>
-      <c r="G14" s="84"/>
-      <c r="H14" s="85" t="s">
+      <c r="G14" s="85"/>
+      <c r="H14" s="86" t="s">
         <v>111</v>
       </c>
-      <c r="I14" s="86" t="s">
+      <c r="I14" s="87" t="s">
         <v>112</v>
       </c>
     </row>
@@ -6322,7 +6301,7 @@
       <c r="B15" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="C15" s="87" t="s">
+      <c r="C15" s="88" t="s">
         <v>53</v>
       </c>
       <c r="D15" s="68"/>
@@ -6332,142 +6311,114 @@
       <c r="F15" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="G15" s="88" t="s">
-        <v>98</v>
-      </c>
-      <c r="H15" s="89" t="s">
+      <c r="G15" s="89"/>
+      <c r="H15" s="90" t="s">
         <v>111</v>
       </c>
-      <c r="I15" s="90" t="s">
+      <c r="I15" s="91" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="91"/>
-      <c r="B16" s="92" t="s">
+      <c r="A16" s="92"/>
+      <c r="B16" s="93" t="s">
         <v>115</v>
       </c>
-      <c r="C16" s="93" t="s">
+      <c r="C16" s="94" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="94"/>
-      <c r="E16" s="95" t="s">
+      <c r="D16" s="95"/>
+      <c r="E16" s="96" t="s">
         <v>95</v>
       </c>
-      <c r="F16" s="96" t="s">
+      <c r="F16" s="97" t="s">
         <v>116</v>
       </c>
-      <c r="G16" s="97" t="s">
-        <v>98</v>
-      </c>
-      <c r="H16" s="98" t="s">
+      <c r="G16" s="98"/>
+      <c r="H16" s="99" t="s">
         <v>111</v>
       </c>
-      <c r="I16" s="99" t="s">
+      <c r="I16" s="100" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="100"/>
+      <c r="A17" s="101"/>
       <c r="B17" s="60" t="s">
-        <v>110</v>
-      </c>
-      <c r="C17" s="101" t="s">
-        <v>59</v>
+        <v>117</v>
+      </c>
+      <c r="C17" s="84" t="s">
+        <v>53</v>
       </c>
       <c r="D17" s="102"/>
-      <c r="E17" s="101" t="s">
+      <c r="E17" s="84" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="103"/>
+      <c r="F17" s="103" t="s">
+        <v>118</v>
+      </c>
       <c r="G17" s="78"/>
       <c r="H17" s="103"/>
       <c r="I17" s="104"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="65"/>
-      <c r="B18" s="66" t="s">
-        <v>117</v>
-      </c>
-      <c r="C18" s="87" t="s">
+      <c r="B18" s="105" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" s="106" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="72"/>
+      <c r="D18" s="107"/>
       <c r="E18" s="67" t="s">
         <v>95</v>
       </c>
       <c r="F18" s="69" t="s">
-        <v>118</v>
-      </c>
-      <c r="G18" s="105" t="s">
-        <v>98</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="G18" s="108"/>
       <c r="H18" s="69"/>
-      <c r="I18" s="106"/>
+      <c r="I18" s="109"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="65"/>
-      <c r="B19" s="107" t="s">
-        <v>119</v>
-      </c>
-      <c r="C19" s="108" t="s">
+      <c r="B19" s="105" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" s="106" t="s">
         <v>53</v>
       </c>
-      <c r="D19" s="109"/>
+      <c r="D19" s="107"/>
       <c r="E19" s="67" t="s">
         <v>95</v>
       </c>
       <c r="F19" s="69" t="s">
-        <v>120</v>
-      </c>
-      <c r="G19" s="105" t="s">
-        <v>98</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="G19" s="108"/>
       <c r="H19" s="69"/>
-      <c r="I19" s="106"/>
+      <c r="I19" s="109"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="65"/>
-      <c r="B20" s="107" t="s">
-        <v>121</v>
-      </c>
-      <c r="C20" s="108" t="s">
+      <c r="A20" s="92"/>
+      <c r="B20" s="93" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" s="94" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="109"/>
-      <c r="E20" s="67" t="s">
+      <c r="D20" s="110"/>
+      <c r="E20" s="96" t="s">
         <v>95</v>
       </c>
-      <c r="F20" s="69" t="s">
-        <v>122</v>
-      </c>
-      <c r="G20" s="105" t="s">
-        <v>98</v>
-      </c>
-      <c r="H20" s="69"/>
-      <c r="I20" s="106"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="91"/>
-      <c r="B21" s="92" t="s">
-        <v>123</v>
-      </c>
-      <c r="C21" s="93" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21" s="110"/>
-      <c r="E21" s="95" t="s">
-        <v>95</v>
-      </c>
-      <c r="F21" s="96" t="s">
+      <c r="F20" s="97" t="s">
         <v>124</v>
       </c>
-      <c r="G21" s="111" t="s">
-        <v>98</v>
-      </c>
-      <c r="H21" s="96"/>
-      <c r="I21" s="112"/>
-    </row>
+      <c r="G20" s="111"/>
+      <c r="H20" s="97"/>
+      <c r="I20" s="112"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -6484,10 +6435,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6585,7 +6536,7 @@
         <v>130</v>
       </c>
       <c r="C6" s="66" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D6" s="72" t="s">
         <v>133</v>
@@ -6601,7 +6552,7 @@
         <v>130</v>
       </c>
       <c r="C7" s="66" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D7" s="72" t="s">
         <v>134</v>
@@ -6619,7 +6570,7 @@
         <v>130</v>
       </c>
       <c r="C8" s="66" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D8" s="72" t="s">
         <v>136</v>
@@ -6635,7 +6586,7 @@
         <v>130</v>
       </c>
       <c r="C9" s="66" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D9" s="72" t="s">
         <v>137</v>
@@ -6651,7 +6602,7 @@
         <v>130</v>
       </c>
       <c r="C10" s="66" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D10" s="72" t="s">
         <v>138</v>
@@ -6667,7 +6618,7 @@
         <v>130</v>
       </c>
       <c r="C11" s="66" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D11" s="72" t="s">
         <v>139</v>
@@ -6683,7 +6634,7 @@
         <v>130</v>
       </c>
       <c r="C12" s="66" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D12" s="72" t="s">
         <v>140</v>
@@ -6699,7 +6650,7 @@
         <v>130</v>
       </c>
       <c r="C13" s="130" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D13" s="131" t="s">
         <v>141</v>
@@ -6717,7 +6668,7 @@
         <v>144</v>
       </c>
       <c r="C14" s="120" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D14" s="60" t="s">
         <v>145</v>
@@ -6748,7 +6699,7 @@
       <c r="B16" s="129" t="s">
         <v>144</v>
       </c>
-      <c r="C16" s="92" t="s">
+      <c r="C16" s="93" t="s">
         <v>115</v>
       </c>
       <c r="D16" s="138" t="s">
@@ -6757,18 +6708,18 @@
       <c r="E16" s="132"/>
       <c r="F16" s="133"/>
     </row>
-    <row r="17" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="134" t="s">
         <v>148</v>
       </c>
       <c r="B17" s="121" t="s">
         <v>149</v>
       </c>
-      <c r="C17" s="120" t="s">
-        <v>110</v>
+      <c r="C17" s="139" t="s">
+        <v>117</v>
       </c>
       <c r="D17" s="60" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="E17" s="122"/>
       <c r="F17" s="62"/>
@@ -6780,11 +6731,11 @@
       <c r="B18" s="124" t="s">
         <v>149</v>
       </c>
-      <c r="C18" s="66" t="s">
-        <v>117</v>
-      </c>
-      <c r="D18" s="72" t="s">
-        <v>150</v>
+      <c r="C18" s="105" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18" s="66" t="s">
+        <v>151</v>
       </c>
       <c r="E18" s="127"/>
       <c r="F18" s="136"/>
@@ -6796,47 +6747,32 @@
       <c r="B19" s="124" t="s">
         <v>149</v>
       </c>
-      <c r="C19" s="107" t="s">
-        <v>119</v>
+      <c r="C19" s="105" t="s">
+        <v>121</v>
       </c>
       <c r="D19" s="66" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E19" s="127"/>
-      <c r="F19" s="136"/>
+      <c r="F19" s="72"/>
     </row>
     <row r="20" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="135" t="s">
+      <c r="A20" s="137" t="s">
         <v>148</v>
       </c>
-      <c r="B20" s="124" t="s">
+      <c r="B20" s="129" t="s">
         <v>149</v>
       </c>
-      <c r="C20" s="107" t="s">
-        <v>121</v>
-      </c>
-      <c r="D20" s="66" t="s">
-        <v>152</v>
-      </c>
-      <c r="E20" s="127"/>
-      <c r="F20" s="72"/>
-    </row>
-    <row r="21" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="137" t="s">
-        <v>148</v>
-      </c>
-      <c r="B21" s="129" t="s">
-        <v>149</v>
-      </c>
-      <c r="C21" s="92" t="s">
+      <c r="C20" s="93" t="s">
         <v>123</v>
       </c>
-      <c r="D21" s="138" t="s">
+      <c r="D20" s="138" t="s">
         <v>153</v>
       </c>
-      <c r="E21" s="132"/>
-      <c r="F21" s="133"/>
-    </row>
+      <c r="E20" s="132"/>
+      <c r="F20" s="133"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -6853,10 +6789,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6875,10 +6811,10 @@
       <c r="B1" s="114"/>
       <c r="C1" s="51"/>
       <c r="D1" s="51"/>
-      <c r="E1" s="139" t="s">
+      <c r="E1" s="140" t="s">
         <v>154</v>
       </c>
-      <c r="F1" s="140" t="s">
+      <c r="F1" s="141" t="s">
         <v>154</v>
       </c>
     </row>
@@ -6887,10 +6823,10 @@
       <c r="B2" s="115"/>
       <c r="C2" s="116"/>
       <c r="D2" s="54"/>
-      <c r="E2" s="141" t="s">
+      <c r="E2" s="142" t="s">
         <v>155</v>
       </c>
-      <c r="F2" s="142" t="s">
+      <c r="F2" s="143" t="s">
         <v>155</v>
       </c>
     </row>
@@ -6918,7 +6854,7 @@
       <c r="A4" s="120" t="s">
         <v>162</v>
       </c>
-      <c r="B4" s="143" t="s">
+      <c r="B4" s="144" t="s">
         <v>163</v>
       </c>
       <c r="C4" s="60" t="s">
@@ -6934,7 +6870,7 @@
       <c r="A5" s="123" t="s">
         <v>162</v>
       </c>
-      <c r="B5" s="144" t="s">
+      <c r="B5" s="145" t="s">
         <v>163</v>
       </c>
       <c r="C5" s="66" t="s">
@@ -6950,13 +6886,13 @@
       <c r="A6" s="123" t="s">
         <v>162</v>
       </c>
-      <c r="B6" s="144" t="s">
+      <c r="B6" s="145" t="s">
         <v>163</v>
       </c>
       <c r="C6" s="66" t="s">
-        <v>99</v>
-      </c>
-      <c r="D6" s="145" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" s="146" t="s">
         <v>166</v>
       </c>
       <c r="E6" s="125"/>
@@ -6966,13 +6902,13 @@
       <c r="A7" s="123" t="s">
         <v>162</v>
       </c>
-      <c r="B7" s="144" t="s">
+      <c r="B7" s="145" t="s">
         <v>163</v>
       </c>
       <c r="C7" s="66" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" s="145" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="146" t="s">
         <v>167</v>
       </c>
       <c r="E7" s="125" t="s">
@@ -6984,13 +6920,13 @@
       <c r="A8" s="123" t="s">
         <v>162</v>
       </c>
-      <c r="B8" s="144" t="s">
+      <c r="B8" s="145" t="s">
         <v>163</v>
       </c>
       <c r="C8" s="66" t="s">
-        <v>102</v>
-      </c>
-      <c r="D8" s="145" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" s="146" t="s">
         <v>169</v>
       </c>
       <c r="E8" s="126"/>
@@ -7000,13 +6936,13 @@
       <c r="A9" s="123" t="s">
         <v>162</v>
       </c>
-      <c r="B9" s="144" t="s">
+      <c r="B9" s="145" t="s">
         <v>163</v>
       </c>
       <c r="C9" s="66" t="s">
-        <v>103</v>
-      </c>
-      <c r="D9" s="145" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9" s="146" t="s">
         <v>170</v>
       </c>
       <c r="E9" s="126"/>
@@ -7016,13 +6952,13 @@
       <c r="A10" s="123" t="s">
         <v>162</v>
       </c>
-      <c r="B10" s="144" t="s">
+      <c r="B10" s="145" t="s">
         <v>163</v>
       </c>
       <c r="C10" s="66" t="s">
-        <v>104</v>
-      </c>
-      <c r="D10" s="145" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="146" t="s">
         <v>171</v>
       </c>
       <c r="E10" s="127"/>
@@ -7032,13 +6968,13 @@
       <c r="A11" s="123" t="s">
         <v>162</v>
       </c>
-      <c r="B11" s="144" t="s">
+      <c r="B11" s="145" t="s">
         <v>163</v>
       </c>
       <c r="C11" s="66" t="s">
-        <v>106</v>
-      </c>
-      <c r="D11" s="145" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="146" t="s">
         <v>172</v>
       </c>
       <c r="E11" s="127"/>
@@ -7048,13 +6984,13 @@
       <c r="A12" s="123" t="s">
         <v>162</v>
       </c>
-      <c r="B12" s="144" t="s">
+      <c r="B12" s="145" t="s">
         <v>163</v>
       </c>
       <c r="C12" s="66" t="s">
-        <v>107</v>
-      </c>
-      <c r="D12" s="145" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="146" t="s">
         <v>173</v>
       </c>
       <c r="E12" s="127"/>
@@ -7064,11 +7000,11 @@
       <c r="A13" s="128" t="s">
         <v>162</v>
       </c>
-      <c r="B13" s="146" t="s">
+      <c r="B13" s="147" t="s">
         <v>163</v>
       </c>
       <c r="C13" s="130" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D13" s="131" t="s">
         <v>174</v>
@@ -7082,13 +7018,13 @@
       <c r="A14" s="134" t="s">
         <v>176</v>
       </c>
-      <c r="B14" s="143" t="s">
+      <c r="B14" s="144" t="s">
         <v>177</v>
       </c>
       <c r="C14" s="120" t="s">
-        <v>110</v>
-      </c>
-      <c r="D14" s="147" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" s="148" t="s">
         <v>178</v>
       </c>
       <c r="E14" s="122"/>
@@ -7098,13 +7034,13 @@
       <c r="A15" s="135" t="s">
         <v>176</v>
       </c>
-      <c r="B15" s="144" t="s">
+      <c r="B15" s="145" t="s">
         <v>177</v>
       </c>
       <c r="C15" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="D15" s="145" t="s">
+      <c r="D15" s="146" t="s">
         <v>179</v>
       </c>
       <c r="E15" s="127"/>
@@ -7114,98 +7050,83 @@
       <c r="A16" s="137" t="s">
         <v>176</v>
       </c>
-      <c r="B16" s="146" t="s">
+      <c r="B16" s="147" t="s">
         <v>177</v>
       </c>
-      <c r="C16" s="92" t="s">
+      <c r="C16" s="93" t="s">
         <v>115</v>
       </c>
-      <c r="D16" s="148" t="s">
+      <c r="D16" s="149" t="s">
         <v>180</v>
       </c>
       <c r="E16" s="132"/>
       <c r="F16" s="133"/>
     </row>
-    <row r="17" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="134" t="s">
         <v>181</v>
       </c>
-      <c r="B17" s="143" t="s">
+      <c r="B17" s="144" t="s">
         <v>182</v>
       </c>
-      <c r="C17" s="120" t="s">
-        <v>110</v>
-      </c>
-      <c r="D17" s="147" t="s">
-        <v>178</v>
+      <c r="C17" s="139" t="s">
+        <v>117</v>
+      </c>
+      <c r="D17" s="148" t="s">
+        <v>183</v>
       </c>
       <c r="E17" s="122"/>
       <c r="F17" s="62"/>
     </row>
     <row r="18" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="135" t="s">
-        <v>181</v>
-      </c>
-      <c r="B18" s="144" t="s">
+        <v>184</v>
+      </c>
+      <c r="B18" s="145" t="s">
         <v>182</v>
       </c>
-      <c r="C18" s="66" t="s">
-        <v>117</v>
-      </c>
-      <c r="D18" s="145" t="s">
-        <v>183</v>
+      <c r="C18" s="105" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18" s="150" t="s">
+        <v>185</v>
       </c>
       <c r="E18" s="127"/>
       <c r="F18" s="136"/>
     </row>
     <row r="19" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="135" t="s">
-        <v>184</v>
-      </c>
-      <c r="B19" s="144" t="s">
+        <v>181</v>
+      </c>
+      <c r="B19" s="145" t="s">
         <v>182</v>
       </c>
-      <c r="C19" s="107" t="s">
-        <v>119</v>
-      </c>
-      <c r="D19" s="149" t="s">
-        <v>185</v>
+      <c r="C19" s="105" t="s">
+        <v>121</v>
+      </c>
+      <c r="D19" s="150" t="s">
+        <v>186</v>
       </c>
       <c r="E19" s="127"/>
-      <c r="F19" s="136"/>
+      <c r="F19" s="72"/>
     </row>
     <row r="20" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="135" t="s">
+      <c r="A20" s="137" t="s">
         <v>181</v>
       </c>
-      <c r="B20" s="144" t="s">
+      <c r="B20" s="147" t="s">
         <v>182</v>
       </c>
-      <c r="C20" s="107" t="s">
-        <v>121</v>
+      <c r="C20" s="93" t="s">
+        <v>123</v>
       </c>
       <c r="D20" s="149" t="s">
-        <v>186</v>
-      </c>
-      <c r="E20" s="127"/>
-      <c r="F20" s="72"/>
-    </row>
-    <row r="21" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="137" t="s">
-        <v>181</v>
-      </c>
-      <c r="B21" s="146" t="s">
-        <v>182</v>
-      </c>
-      <c r="C21" s="92" t="s">
-        <v>123</v>
-      </c>
-      <c r="D21" s="148" t="s">
         <v>187</v>
       </c>
-      <c r="E21" s="132"/>
-      <c r="F21" s="133"/>
-    </row>
+      <c r="E20" s="132"/>
+      <c r="F20" s="133"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Parse OCA XLS(X) files based on column name
</commit_message>
<xml_diff>
--- a/tests/assets/oca_template.xlsx
+++ b/tests/assets/oca_template.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="198">
   <si>
     <t xml:space="preserve">OCA DATA CAPTURE SPECIFICATION</t>
   </si>
@@ -806,10 +806,31 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">OL: Conditional [Condition]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OL: Conditional [Dependencies]</t>
+    <t xml:space="preserve">CB-CL: Classification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CB-AN: Attribute Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CB-AT: Attribute Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CB-FA: Flagged Attribute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OL-CH: Character Encoding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OL-FT: Format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OL-EC: Entry Codes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OL-CC: Conditional [Condition]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OL-CD: Conditional [Dependencies]</t>
   </si>
   <si>
     <t xml:space="preserve">projectName</t>
@@ -911,10 +932,19 @@
     <t xml:space="preserve">Claim</t>
   </si>
   <si>
-    <t xml:space="preserve">OL: Meta [Form Name]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OL: Meta [Form Description]</t>
+    <t xml:space="preserve">OL-MN: Meta [Form Name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OL-MD: Meta [Form Description]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OL-LA: Label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OL-EN: Entry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OL-IN: Information</t>
   </si>
   <si>
     <t xml:space="preserve">HCF Project Onboarding Form</t>
@@ -1006,7 +1036,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">OL: </t>
+      <t xml:space="preserve">OL-MN: </t>
     </r>
     <r>
       <rPr>
@@ -1014,7 +1044,6 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">元 </t>
     </r>
@@ -1034,7 +1063,6 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">表格名称</t>
     </r>
@@ -1058,7 +1086,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">OL: </t>
+      <t xml:space="preserve">OL-MD: </t>
     </r>
     <r>
       <rPr>
@@ -1066,7 +1094,6 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">元 </t>
     </r>
@@ -1086,7 +1113,6 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">表格说明</t>
     </r>
@@ -1110,7 +1136,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">CB: </t>
+      <t xml:space="preserve">CB-AT: </t>
     </r>
     <r>
       <rPr>
@@ -1118,7 +1144,6 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">属性名</t>
     </r>
@@ -1132,7 +1157,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">OL: </t>
+      <t xml:space="preserve">OL-LA: </t>
     </r>
     <r>
       <rPr>
@@ -1140,7 +1165,6 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">标签</t>
     </r>
@@ -1154,7 +1178,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">OL: </t>
+      <t xml:space="preserve">OL-EN: </t>
     </r>
     <r>
       <rPr>
@@ -1162,7 +1186,6 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">条目</t>
     </r>
@@ -1176,7 +1199,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">OL: </t>
+      <t xml:space="preserve">OL-IN: </t>
     </r>
     <r>
       <rPr>
@@ -1184,7 +1207,6 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">信息</t>
     </r>
@@ -2298,10 +2320,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="[$-F800]DDDD&quot;, &quot;MMMM\ DD&quot;, &quot;YYYY"/>
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd&quot;, &quot;mmmm\ dd&quot;, &quot;yyyy"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="10"/>
       <name val="Helvetica Neue"/>
@@ -2479,6 +2501,12 @@
       <name val="Noto Sans CJK SC"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Noto Sans CJK SC"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -3697,44 +3725,44 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="25" fillId="10" borderId="49" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="26" fillId="10" borderId="49" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="25" fillId="10" borderId="51" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="26" fillId="10" borderId="51" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="25" fillId="10" borderId="53" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="10" borderId="53" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="21"/>
+    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
   <dxfs count="54">
     <dxf>
@@ -4352,9 +4380,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>122400</xdr:colOff>
+      <xdr:colOff>122040</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>89640</xdr:rowOff>
+      <xdr:rowOff>89280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4367,13 +4395,13 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4060440" y="281880"/>
-          <a:ext cx="2903400" cy="823680"/>
+          <a:off x="4060800" y="282240"/>
+          <a:ext cx="2902680" cy="822960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -4384,25 +4412,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:D66"/>
+  <dimension ref="B1:D980"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="3:3 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="46.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="35.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="91.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="5" style="1" width="8.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="1" width="14.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="1" width="14.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5843,174 +5871,282 @@
     <mergeCell ref="B65:D65"/>
   </mergeCells>
   <conditionalFormatting sqref="F21:F40">
-    <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="0"/>
+    <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="0">
+      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",F21)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21:F40">
-    <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="1"/>
+    <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="1">
+      <formula>NOT(ISERROR(SEARCH("OPTIONAL",F21)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21:F40">
-    <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="2"/>
+    <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="2">
+      <formula>NOT(ISERROR(SEARCH("REQUIRED",F21)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63 C66:C980">
-    <cfRule type="containsText" priority="5" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="3"/>
+    <cfRule type="containsText" priority="5" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="3">
+      <formula>NOT(ISERROR(SEARCH("CONDITIONAL",C63)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63 C66:C980">
-    <cfRule type="containsText" priority="6" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="4"/>
+    <cfRule type="containsText" priority="6" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="4">
+      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C63)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63 C66:C980">
-    <cfRule type="containsText" priority="7" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="5"/>
+    <cfRule type="containsText" priority="7" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="5">
+      <formula>NOT(ISERROR(SEARCH("OPTIONAL",C63)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63 C66:C980">
-    <cfRule type="containsText" priority="8" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="6"/>
+    <cfRule type="containsText" priority="8" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="6">
+      <formula>NOT(ISERROR(SEARCH("REQUIRED",C63)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" priority="9" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="7"/>
+    <cfRule type="containsText" priority="9" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="7">
+      <formula>NOT(ISERROR(SEARCH("CONDITIONAL",C41)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" priority="10" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="8"/>
+    <cfRule type="containsText" priority="10" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="8">
+      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C41)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" priority="11" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="9"/>
+    <cfRule type="containsText" priority="11" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="9">
+      <formula>NOT(ISERROR(SEARCH("OPTIONAL",C41)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" priority="12" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="10"/>
+    <cfRule type="containsText" priority="12" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="10">
+      <formula>NOT(ISERROR(SEARCH("REQUIRED",C41)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="containsText" priority="13" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="11"/>
+    <cfRule type="containsText" priority="13" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="11">
+      <formula>NOT(ISERROR(SEARCH("CONDITIONAL",C24)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="containsText" priority="14" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="12"/>
+    <cfRule type="containsText" priority="14" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="12">
+      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C24)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="containsText" priority="15" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="13"/>
+    <cfRule type="containsText" priority="15" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="13">
+      <formula>NOT(ISERROR(SEARCH("OPTIONAL",C24)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="containsText" priority="16" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="14"/>
+    <cfRule type="containsText" priority="16" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="14">
+      <formula>NOT(ISERROR(SEARCH("REQUIRED",C24)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C27">
-    <cfRule type="containsText" priority="17" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="15"/>
+    <cfRule type="containsText" priority="17" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="15">
+      <formula>NOT(ISERROR(SEARCH("CONDITIONAL",C25)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C27">
-    <cfRule type="containsText" priority="18" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="16"/>
+    <cfRule type="containsText" priority="18" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="16">
+      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C25)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C27">
-    <cfRule type="containsText" priority="19" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="17"/>
+    <cfRule type="containsText" priority="19" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="17">
+      <formula>NOT(ISERROR(SEARCH("OPTIONAL",C25)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C27">
-    <cfRule type="containsText" priority="20" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="18"/>
+    <cfRule type="containsText" priority="20" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="18">
+      <formula>NOT(ISERROR(SEARCH("REQUIRED",C25)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C23">
-    <cfRule type="containsText" priority="21" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="19"/>
+    <cfRule type="containsText" priority="21" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="19">
+      <formula>NOT(ISERROR(SEARCH("CONDITIONAL",C22)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C23">
-    <cfRule type="containsText" priority="22" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="20"/>
+    <cfRule type="containsText" priority="22" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="20">
+      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C22)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C23">
-    <cfRule type="containsText" priority="23" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="21"/>
+    <cfRule type="containsText" priority="23" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="21">
+      <formula>NOT(ISERROR(SEARCH("OPTIONAL",C22)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C23">
-    <cfRule type="containsText" priority="24" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="22"/>
+    <cfRule type="containsText" priority="24" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="22">
+      <formula>NOT(ISERROR(SEARCH("REQUIRED",C22)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="containsText" priority="25" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="23"/>
+    <cfRule type="containsText" priority="25" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="23">
+      <formula>NOT(ISERROR(SEARCH("CONDITIONAL",C30)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="containsText" priority="26" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="24"/>
+    <cfRule type="containsText" priority="26" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="24">
+      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C30)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="containsText" priority="27" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="25"/>
+    <cfRule type="containsText" priority="27" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="25">
+      <formula>NOT(ISERROR(SEARCH("OPTIONAL",C30)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="containsText" priority="28" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="26"/>
+    <cfRule type="containsText" priority="28" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="26">
+      <formula>NOT(ISERROR(SEARCH("REQUIRED",C30)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="containsText" priority="29" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="27"/>
+    <cfRule type="containsText" priority="29" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="27">
+      <formula>NOT(ISERROR(SEARCH("CONDITIONAL",C31)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="containsText" priority="30" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="28"/>
+    <cfRule type="containsText" priority="30" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="28">
+      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C31)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="containsText" priority="31" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="29"/>
+    <cfRule type="containsText" priority="31" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="29">
+      <formula>NOT(ISERROR(SEARCH("OPTIONAL",C31)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="containsText" priority="32" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="30"/>
+    <cfRule type="containsText" priority="32" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="30">
+      <formula>NOT(ISERROR(SEARCH("REQUIRED",C31)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="containsText" priority="33" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="31"/>
+    <cfRule type="containsText" priority="33" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="31">
+      <formula>NOT(ISERROR(SEARCH("CONDITIONAL",C32)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="containsText" priority="34" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="32"/>
+    <cfRule type="containsText" priority="34" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="32">
+      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C32)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="containsText" priority="35" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="33"/>
+    <cfRule type="containsText" priority="35" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="33">
+      <formula>NOT(ISERROR(SEARCH("OPTIONAL",C32)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="containsText" priority="36" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="34"/>
+    <cfRule type="containsText" priority="36" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="34">
+      <formula>NOT(ISERROR(SEARCH("REQUIRED",C32)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42:C43">
-    <cfRule type="containsText" priority="37" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="35"/>
+    <cfRule type="containsText" priority="37" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="35">
+      <formula>NOT(ISERROR(SEARCH("CONDITIONAL",C42)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42:C43">
-    <cfRule type="containsText" priority="38" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="36"/>
+    <cfRule type="containsText" priority="38" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="36">
+      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C42)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42:C43">
-    <cfRule type="containsText" priority="39" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="37"/>
+    <cfRule type="containsText" priority="39" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="37">
+      <formula>NOT(ISERROR(SEARCH("OPTIONAL",C42)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42:C43">
-    <cfRule type="containsText" priority="40" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="38"/>
+    <cfRule type="containsText" priority="40" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="38">
+      <formula>NOT(ISERROR(SEARCH("REQUIRED",C42)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33:C40 C21 C44:C48">
-    <cfRule type="containsText" priority="41" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="39"/>
+    <cfRule type="containsText" priority="41" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="39">
+      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C21)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33:C40 C21 C44:C48">
-    <cfRule type="containsText" priority="42" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="40"/>
+    <cfRule type="containsText" priority="42" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="40">
+      <formula>NOT(ISERROR(SEARCH("OPTIONAL",C21)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33:C40 C21 C44:C48">
-    <cfRule type="containsText" priority="43" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="41"/>
+    <cfRule type="containsText" priority="43" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="41">
+      <formula>NOT(ISERROR(SEARCH("REQUIRED",C21)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:C17 C33:C40 C21 C44:C48">
-    <cfRule type="containsText" priority="44" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="42"/>
+    <cfRule type="containsText" priority="44" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="42">
+      <formula>NOT(ISERROR(SEARCH("CONDITIONAL",C16)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:C17">
-    <cfRule type="containsText" priority="45" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="43"/>
+    <cfRule type="containsText" priority="45" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="43">
+      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C16)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:C17">
-    <cfRule type="containsText" priority="46" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="44"/>
+    <cfRule type="containsText" priority="46" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="44">
+      <formula>NOT(ISERROR(SEARCH("OPTIONAL",C16)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:C17">
-    <cfRule type="containsText" priority="47" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="45"/>
+    <cfRule type="containsText" priority="47" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="45">
+      <formula>NOT(ISERROR(SEARCH("REQUIRED",C16)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" priority="48" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="46"/>
+    <cfRule type="containsText" priority="48" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="46">
+      <formula>NOT(ISERROR(SEARCH("CONDITIONAL",C29)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" priority="49" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="47"/>
+    <cfRule type="containsText" priority="49" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="47">
+      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C29)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" priority="50" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="48"/>
+    <cfRule type="containsText" priority="50" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="48">
+      <formula>NOT(ISERROR(SEARCH("OPTIONAL",C29)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" priority="51" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="49"/>
+    <cfRule type="containsText" priority="51" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="49">
+      <formula>NOT(ISERROR(SEARCH("REQUIRED",C29)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="containsText" priority="52" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="50"/>
+    <cfRule type="containsText" priority="52" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="CONDITIONAL" dxfId="50">
+      <formula>NOT(ISERROR(SEARCH("CONDITIONAL",C28)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="containsText" priority="53" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="51"/>
+    <cfRule type="containsText" priority="53" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="NOT NEEDED" dxfId="51">
+      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C28)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="containsText" priority="54" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="52"/>
+    <cfRule type="containsText" priority="54" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="OPTIONAL" dxfId="52">
+      <formula>NOT(ISERROR(SEARCH("OPTIONAL",C28)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="containsText" priority="55" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="53"/>
+    <cfRule type="containsText" priority="55" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="REQUIRED" dxfId="53">
+      <formula>NOT(ISERROR(SEARCH("REQUIRED",C28)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C11" r:id="rId1" display="paul.knowles@humancolossus.org"/>
     <hyperlink ref="B64" r:id="rId2" display="© The Human Colossus Foundation 2021. Some rights reserved. This work is available under the CC BY-NC-SA 3.0 IGO licence."/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -6020,17 +6156,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="3:3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.66"/>
@@ -6041,7 +6177,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="28.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="10.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6062,46 +6197,46 @@
       <c r="F2" s="55"/>
       <c r="G2" s="54"/>
     </row>
-    <row r="3" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="56" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
       <c r="B3" s="56" t="s">
-        <v>20</v>
+        <v>93</v>
       </c>
       <c r="C3" s="57" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
       <c r="D3" s="56" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="E3" s="57" t="s">
-        <v>27</v>
+        <v>96</v>
       </c>
       <c r="F3" s="58" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="G3" s="56" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="H3" s="56" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="I3" s="56" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="59"/>
       <c r="B4" s="60" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="C4" s="61" t="s">
         <v>53</v>
       </c>
       <c r="D4" s="62"/>
       <c r="E4" s="61" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="F4" s="63"/>
       <c r="G4" s="64"/>
@@ -6111,17 +6246,17 @@
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="65"/>
       <c r="B5" s="66" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C5" s="67" t="s">
         <v>53</v>
       </c>
       <c r="D5" s="68"/>
       <c r="E5" s="67" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="F5" s="69" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="G5" s="70"/>
       <c r="H5" s="69"/>
@@ -6130,14 +6265,14 @@
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="65"/>
       <c r="B6" s="66" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="C6" s="67" t="s">
         <v>53</v>
       </c>
       <c r="D6" s="72"/>
       <c r="E6" s="67" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="F6" s="69"/>
       <c r="G6" s="73"/>
@@ -6147,18 +6282,18 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="65"/>
       <c r="B7" s="66" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="C7" s="67" t="s">
         <v>53</v>
       </c>
       <c r="D7" s="72"/>
       <c r="E7" s="67" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="F7" s="69"/>
       <c r="G7" s="64" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="H7" s="69"/>
       <c r="I7" s="72"/>
@@ -6166,14 +6301,14 @@
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="65"/>
       <c r="B8" s="66" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="C8" s="75" t="s">
         <v>53</v>
       </c>
       <c r="D8" s="72"/>
       <c r="E8" s="67" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="F8" s="69"/>
       <c r="G8" s="64"/>
@@ -6183,17 +6318,17 @@
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="65"/>
       <c r="B9" s="66" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="C9" s="75" t="s">
         <v>53</v>
       </c>
       <c r="D9" s="72"/>
       <c r="E9" s="67" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="F9" s="69" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="G9" s="76"/>
       <c r="H9" s="69"/>
@@ -6202,16 +6337,16 @@
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="65"/>
       <c r="B10" s="66" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="C10" s="75" t="s">
         <v>53</v>
       </c>
       <c r="D10" s="72" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="E10" s="67" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="F10" s="69"/>
       <c r="G10" s="64"/>
@@ -6221,16 +6356,16 @@
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="65"/>
       <c r="B11" s="66" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="C11" s="67" t="s">
         <v>53</v>
       </c>
       <c r="D11" s="72" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="E11" s="67" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="F11" s="69"/>
       <c r="G11" s="64"/>
@@ -6240,16 +6375,16 @@
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="65"/>
       <c r="B12" s="66" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="C12" s="67" t="s">
         <v>53</v>
       </c>
       <c r="D12" s="72" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="E12" s="67" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="F12" s="69"/>
       <c r="G12" s="78"/>
@@ -6259,18 +6394,18 @@
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="65"/>
       <c r="B13" s="66" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C13" s="67" t="s">
         <v>53</v>
       </c>
       <c r="D13" s="72"/>
       <c r="E13" s="67" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="F13" s="69"/>
       <c r="G13" s="80" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="H13" s="81"/>
       <c r="I13" s="82"/>
@@ -6278,84 +6413,84 @@
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="83"/>
       <c r="B14" s="60" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="C14" s="84" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="D14" s="62"/>
       <c r="E14" s="61" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="F14" s="63"/>
       <c r="G14" s="85"/>
       <c r="H14" s="86" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="I14" s="87" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="65"/>
       <c r="B15" s="66" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="C15" s="88" t="s">
         <v>53</v>
       </c>
       <c r="D15" s="68"/>
       <c r="E15" s="67" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="F15" s="69" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="G15" s="89"/>
       <c r="H15" s="90" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="I15" s="91" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="92"/>
       <c r="B16" s="93" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="C16" s="94" t="s">
         <v>53</v>
       </c>
       <c r="D16" s="95"/>
       <c r="E16" s="96" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="F16" s="97" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="G16" s="98"/>
       <c r="H16" s="99" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="I16" s="100" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="101"/>
       <c r="B17" s="60" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="C17" s="84" t="s">
         <v>53</v>
       </c>
       <c r="D17" s="102"/>
       <c r="E17" s="84" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="F17" s="103" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="G17" s="78"/>
       <c r="H17" s="103"/>
@@ -6364,17 +6499,17 @@
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="65"/>
       <c r="B18" s="105" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="C18" s="106" t="s">
         <v>53</v>
       </c>
       <c r="D18" s="107"/>
       <c r="E18" s="67" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="F18" s="69" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="G18" s="108"/>
       <c r="H18" s="69"/>
@@ -6383,17 +6518,17 @@
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="65"/>
       <c r="B19" s="105" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="C19" s="106" t="s">
         <v>53</v>
       </c>
       <c r="D19" s="107"/>
       <c r="E19" s="67" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="F19" s="69" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="G19" s="108"/>
       <c r="H19" s="69"/>
@@ -6402,17 +6537,17 @@
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="92"/>
       <c r="B20" s="93" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="C20" s="94" t="s">
         <v>53</v>
       </c>
       <c r="D20" s="110"/>
       <c r="E20" s="96" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="F20" s="97" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="G20" s="111"/>
       <c r="H20" s="97"/>
@@ -6421,8 +6556,8 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -6431,17 +6566,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="3:3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="48.17"/>
@@ -6449,7 +6584,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="41.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="47.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="57.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="10.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6458,10 +6592,10 @@
       <c r="C1" s="51"/>
       <c r="D1" s="51"/>
       <c r="E1" s="56" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="F1" s="57" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6470,304 +6604,304 @@
       <c r="C2" s="116"/>
       <c r="D2" s="54"/>
       <c r="E2" s="117" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="F2" s="118" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="119" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B3" s="119" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="C3" s="117" t="s">
-        <v>20</v>
+        <v>93</v>
       </c>
       <c r="D3" s="117" t="s">
-        <v>41</v>
+        <v>136</v>
       </c>
       <c r="E3" s="56" t="s">
-        <v>44</v>
+        <v>137</v>
       </c>
       <c r="F3" s="57" t="s">
-        <v>47</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="120" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="B4" s="121" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C4" s="60" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="D4" s="62" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="E4" s="122"/>
       <c r="F4" s="62"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="123" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="B5" s="124" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C5" s="66" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="D5" s="72" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="E5" s="125"/>
       <c r="F5" s="72"/>
     </row>
     <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="123" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="B6" s="124" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C6" s="66" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D6" s="72" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="E6" s="125"/>
       <c r="F6" s="72"/>
     </row>
     <row r="7" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="123" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="B7" s="124" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C7" s="66" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="D7" s="72" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="E7" s="125" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="F7" s="72"/>
     </row>
     <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="123" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="B8" s="124" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C8" s="66" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="D8" s="72" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="E8" s="126"/>
       <c r="F8" s="74"/>
     </row>
     <row r="9" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="123" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="B9" s="124" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C9" s="66" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="D9" s="72" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="E9" s="126"/>
       <c r="F9" s="74"/>
     </row>
     <row r="10" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="123" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="B10" s="124" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C10" s="66" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="D10" s="72" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="E10" s="127"/>
       <c r="F10" s="72"/>
     </row>
     <row r="11" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="123" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="B11" s="124" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C11" s="66" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="D11" s="72" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="E11" s="127"/>
       <c r="F11" s="72"/>
     </row>
     <row r="12" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="123" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="B12" s="124" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C12" s="66" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="D12" s="72" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="E12" s="127"/>
       <c r="F12" s="72"/>
     </row>
     <row r="13" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="128" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="B13" s="129" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C13" s="130" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="D13" s="131" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="E13" s="132" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="F13" s="133"/>
     </row>
     <row r="14" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="134" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="B14" s="121" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="C14" s="120" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="D14" s="60" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="E14" s="122"/>
       <c r="F14" s="62"/>
     </row>
     <row r="15" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="135" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="B15" s="124" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="C15" s="66" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="D15" s="72" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="E15" s="127"/>
       <c r="F15" s="136"/>
     </row>
     <row r="16" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="137" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="B16" s="129" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="C16" s="93" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="D16" s="138" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="E16" s="132"/>
       <c r="F16" s="133"/>
     </row>
     <row r="17" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="134" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="B17" s="121" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="C17" s="139" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="D17" s="60" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="E17" s="122"/>
       <c r="F17" s="62"/>
     </row>
     <row r="18" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="135" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="B18" s="124" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="C18" s="105" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="D18" s="66" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="E18" s="127"/>
       <c r="F18" s="136"/>
     </row>
     <row r="19" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="135" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="B19" s="124" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="C19" s="105" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="D19" s="66" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="E19" s="127"/>
       <c r="F19" s="72"/>
     </row>
     <row r="20" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="137" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="B20" s="129" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="C20" s="93" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="D20" s="138" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="E20" s="132"/>
       <c r="F20" s="133"/>
@@ -6775,8 +6909,8 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -6785,17 +6919,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="3:3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="51.17"/>
@@ -6803,7 +6937,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="43.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="49.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="10.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6812,10 +6945,10 @@
       <c r="C1" s="51"/>
       <c r="D1" s="51"/>
       <c r="E1" s="140" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="F1" s="141" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6824,304 +6957,304 @@
       <c r="C2" s="116"/>
       <c r="D2" s="54"/>
       <c r="E2" s="142" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="F2" s="143" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="119" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="B3" s="119" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="C3" s="117" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="D3" s="117" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="E3" s="56" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="F3" s="57" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="120" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="B4" s="144" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="C4" s="60" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="D4" s="62" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="E4" s="122"/>
       <c r="F4" s="62"/>
     </row>
     <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="123" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="B5" s="145" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="C5" s="66" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="D5" s="72" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="E5" s="125"/>
       <c r="F5" s="72"/>
     </row>
     <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="123" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="B6" s="145" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="C6" s="66" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D6" s="146" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="E6" s="125"/>
       <c r="F6" s="72"/>
     </row>
     <row r="7" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="123" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="B7" s="145" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="C7" s="66" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="D7" s="146" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="E7" s="125" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="F7" s="72"/>
     </row>
     <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="123" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="B8" s="145" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="C8" s="66" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="D8" s="146" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="E8" s="126"/>
       <c r="F8" s="74"/>
     </row>
     <row r="9" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="123" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="B9" s="145" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="C9" s="66" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="D9" s="146" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="E9" s="126"/>
       <c r="F9" s="74"/>
     </row>
     <row r="10" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="123" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="B10" s="145" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="C10" s="66" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="D10" s="146" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="E10" s="127"/>
       <c r="F10" s="72"/>
     </row>
     <row r="11" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="123" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="B11" s="145" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="C11" s="66" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="D11" s="146" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="E11" s="127"/>
       <c r="F11" s="72"/>
     </row>
     <row r="12" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="123" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="B12" s="145" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="C12" s="66" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="D12" s="146" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="E12" s="127"/>
       <c r="F12" s="72"/>
     </row>
     <row r="13" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="128" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="B13" s="147" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="C13" s="130" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="D13" s="131" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="E13" s="132" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="F13" s="133"/>
     </row>
     <row r="14" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="134" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="B14" s="144" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="C14" s="120" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="D14" s="148" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="E14" s="122"/>
       <c r="F14" s="62"/>
     </row>
     <row r="15" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="135" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="B15" s="145" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="C15" s="66" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="D15" s="146" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="E15" s="127"/>
       <c r="F15" s="136"/>
     </row>
     <row r="16" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="137" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="B16" s="147" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="C16" s="93" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="D16" s="149" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="E16" s="132"/>
       <c r="F16" s="133"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="134" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="B17" s="144" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="C17" s="139" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="D17" s="148" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="E17" s="122"/>
       <c r="F17" s="62"/>
     </row>
     <row r="18" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="135" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="B18" s="145" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="C18" s="105" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="D18" s="150" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="E18" s="127"/>
       <c r="F18" s="136"/>
     </row>
     <row r="19" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="135" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="B19" s="145" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="C19" s="105" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="D19" s="150" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="E19" s="127"/>
       <c r="F19" s="72"/>
     </row>
     <row r="20" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="137" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="B20" s="147" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="C20" s="93" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="D20" s="149" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="E20" s="132"/>
       <c r="F20" s="133"/>
@@ -7129,8 +7262,8 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Handle 'CB-RS: Reference SAI' column in XLS parser
</commit_message>
<xml_diff>
--- a/tests/assets/oca_template.xlsx
+++ b/tests/assets/oca_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="READ ME" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="200">
   <si>
     <t xml:space="preserve">OCA DATA CAPTURE SPECIFICATION</t>
   </si>
@@ -815,6 +815,9 @@
     <t xml:space="preserve">CB-AT: Attribute Type</t>
   </si>
   <si>
+    <t xml:space="preserve">CB-RS: Reference SAI</t>
+  </si>
+  <si>
     <t xml:space="preserve">CB-FA: Flagged Attribute</t>
   </si>
   <si>
@@ -881,7 +884,10 @@
     <t xml:space="preserve">linkedForm</t>
   </si>
   <si>
-    <t xml:space="preserve">SAI:linkedFormSAI</t>
+    <t xml:space="preserve">Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linkedFormSAI</t>
   </si>
   <si>
     <t xml:space="preserve">${0}==‘LEI’ || ${1}==‘SHAP’</t>
@@ -1044,6 +1050,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">元 </t>
     </r>
@@ -1063,6 +1070,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">表格名称</t>
     </r>
@@ -1094,6 +1102,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">元 </t>
     </r>
@@ -1113,6 +1122,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">表格说明</t>
     </r>
@@ -1144,6 +1154,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">属性名</t>
     </r>
@@ -1165,6 +1176,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">标签</t>
     </r>
@@ -1186,6 +1198,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">条目</t>
     </r>
@@ -1207,6 +1220,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">信息</t>
     </r>
@@ -2323,7 +2337,7 @@
     <numFmt numFmtId="165" formatCode="[$-F800]dddd&quot;, &quot;mmmm\ dd&quot;, &quot;yyyy"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="27">
     <font>
       <sz val="10"/>
       <name val="Helvetica Neue"/>
@@ -2501,12 +2515,6 @@
       <name val="Noto Sans CJK SC"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Noto Sans CJK SC"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -3725,31 +3733,31 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="26" fillId="10" borderId="49" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="25" fillId="10" borderId="49" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="26" fillId="10" borderId="51" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="25" fillId="10" borderId="51" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="10" borderId="53" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="25" fillId="10" borderId="53" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4380,9 +4388,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>122040</xdr:colOff>
+      <xdr:colOff>121680</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>89280</xdr:rowOff>
+      <xdr:rowOff>88920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4396,7 +4404,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4060800" y="282240"/>
-          <a:ext cx="2902680" cy="822960"/>
+          <a:ext cx="2902320" cy="822600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4420,7 +4428,7 @@
   <dimension ref="B1:D980"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="3:3 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6160,10 +6168,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1048576"/>
+  <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="3:3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6171,12 +6179,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="28.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="28.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6185,8 +6193,9 @@
       <c r="C1" s="51"/>
       <c r="D1" s="51"/>
       <c r="E1" s="51"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="51"/>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="53"/>
@@ -6194,10 +6203,11 @@
       <c r="C2" s="54"/>
       <c r="D2" s="54"/>
       <c r="E2" s="54"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="54"/>
-    </row>
-    <row r="3" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F2" s="54"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="54"/>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="56" t="s">
         <v>92</v>
       </c>
@@ -6207,16 +6217,16 @@
       <c r="C3" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="E3" s="57" t="s">
+      <c r="E3" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="F3" s="58" t="s">
+      <c r="F3" s="57" t="s">
         <v>97</v>
       </c>
-      <c r="G3" s="56" t="s">
+      <c r="G3" s="58" t="s">
         <v>98</v>
       </c>
       <c r="H3" s="56" t="s">
@@ -6224,334 +6234,356 @@
       </c>
       <c r="I3" s="56" t="s">
         <v>100</v>
+      </c>
+      <c r="J3" s="56" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="59"/>
       <c r="B4" s="60" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C4" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="62"/>
-      <c r="E4" s="61" t="s">
-        <v>102</v>
-      </c>
-      <c r="F4" s="63"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="63"/>
-      <c r="I4" s="62"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="61" t="s">
+        <v>103</v>
+      </c>
+      <c r="G4" s="63"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="62"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="65"/>
       <c r="B5" s="66" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C5" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="68"/>
-      <c r="E5" s="67" t="s">
-        <v>102</v>
-      </c>
-      <c r="F5" s="69" t="s">
-        <v>104</v>
-      </c>
-      <c r="G5" s="70"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="71"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="G5" s="69" t="s">
+        <v>105</v>
+      </c>
+      <c r="H5" s="70"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="71"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="65"/>
       <c r="B6" s="66" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C6" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="72"/>
-      <c r="E6" s="67" t="s">
-        <v>102</v>
-      </c>
-      <c r="F6" s="69"/>
-      <c r="G6" s="73"/>
-      <c r="H6" s="69"/>
-      <c r="I6" s="74"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="G6" s="69"/>
+      <c r="H6" s="73"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="74"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="65"/>
       <c r="B7" s="66" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C7" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="72"/>
-      <c r="E7" s="67" t="s">
-        <v>102</v>
-      </c>
-      <c r="F7" s="69"/>
-      <c r="G7" s="64" t="s">
-        <v>107</v>
-      </c>
-      <c r="H7" s="69"/>
-      <c r="I7" s="72"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="G7" s="69"/>
+      <c r="H7" s="64" t="s">
+        <v>108</v>
+      </c>
+      <c r="I7" s="69"/>
+      <c r="J7" s="72"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="65"/>
       <c r="B8" s="66" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C8" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="72"/>
-      <c r="E8" s="67" t="s">
-        <v>102</v>
-      </c>
-      <c r="F8" s="69"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="69"/>
-      <c r="I8" s="72"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="G8" s="69"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="72"/>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="65"/>
       <c r="B9" s="66" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C9" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="72"/>
-      <c r="E9" s="67" t="s">
-        <v>102</v>
-      </c>
-      <c r="F9" s="69" t="s">
-        <v>104</v>
-      </c>
-      <c r="G9" s="76"/>
-      <c r="H9" s="69"/>
-      <c r="I9" s="77"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="G9" s="69" t="s">
+        <v>105</v>
+      </c>
+      <c r="H9" s="76"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="77"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="65"/>
       <c r="B10" s="66" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C10" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="72" t="s">
-        <v>111</v>
-      </c>
-      <c r="E10" s="67" t="s">
-        <v>102</v>
-      </c>
-      <c r="F10" s="69"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="69"/>
-      <c r="I10" s="72"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="72" t="s">
+        <v>112</v>
+      </c>
+      <c r="F10" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10" s="69"/>
+      <c r="H10" s="64"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="72"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="65"/>
       <c r="B11" s="66" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C11" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="72" t="s">
-        <v>111</v>
-      </c>
-      <c r="E11" s="67" t="s">
-        <v>102</v>
-      </c>
-      <c r="F11" s="69"/>
-      <c r="G11" s="64"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="72"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="72" t="s">
+        <v>112</v>
+      </c>
+      <c r="F11" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="G11" s="69"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="69"/>
+      <c r="J11" s="72"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="65"/>
       <c r="B12" s="66" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C12" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="72" t="s">
-        <v>111</v>
-      </c>
-      <c r="E12" s="67" t="s">
-        <v>102</v>
-      </c>
-      <c r="F12" s="69"/>
-      <c r="G12" s="78"/>
-      <c r="H12" s="69"/>
-      <c r="I12" s="79"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="72" t="s">
+        <v>112</v>
+      </c>
+      <c r="F12" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="G12" s="69"/>
+      <c r="H12" s="78"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="79"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="65"/>
       <c r="B13" s="66" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C13" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="72"/>
-      <c r="E13" s="67" t="s">
-        <v>102</v>
-      </c>
-      <c r="F13" s="69"/>
-      <c r="G13" s="80" t="s">
-        <v>115</v>
-      </c>
-      <c r="H13" s="81"/>
-      <c r="I13" s="82"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="G13" s="69"/>
+      <c r="H13" s="80" t="s">
+        <v>116</v>
+      </c>
+      <c r="I13" s="81"/>
+      <c r="J13" s="82"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="83"/>
       <c r="B14" s="60" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C14" s="84" t="s">
-        <v>117</v>
-      </c>
-      <c r="D14" s="62"/>
-      <c r="E14" s="61" t="s">
-        <v>102</v>
-      </c>
-      <c r="F14" s="63"/>
-      <c r="G14" s="85"/>
-      <c r="H14" s="86" t="s">
         <v>118</v>
       </c>
-      <c r="I14" s="87" t="s">
+      <c r="D14" s="84" t="s">
         <v>119</v>
+      </c>
+      <c r="E14" s="62"/>
+      <c r="F14" s="61" t="s">
+        <v>103</v>
+      </c>
+      <c r="G14" s="63"/>
+      <c r="H14" s="85"/>
+      <c r="I14" s="86" t="s">
+        <v>120</v>
+      </c>
+      <c r="J14" s="87" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="65"/>
       <c r="B15" s="66" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C15" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="68"/>
-      <c r="E15" s="67" t="s">
-        <v>102</v>
-      </c>
-      <c r="F15" s="69" t="s">
+      <c r="D15" s="88"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="G15" s="69" t="s">
+        <v>123</v>
+      </c>
+      <c r="H15" s="89"/>
+      <c r="I15" s="90" t="s">
+        <v>120</v>
+      </c>
+      <c r="J15" s="91" t="s">
         <v>121</v>
-      </c>
-      <c r="G15" s="89"/>
-      <c r="H15" s="90" t="s">
-        <v>118</v>
-      </c>
-      <c r="I15" s="91" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="92"/>
       <c r="B16" s="93" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C16" s="94" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="95"/>
-      <c r="E16" s="96" t="s">
-        <v>102</v>
-      </c>
-      <c r="F16" s="97" t="s">
-        <v>123</v>
-      </c>
-      <c r="G16" s="98"/>
-      <c r="H16" s="99" t="s">
-        <v>118</v>
-      </c>
-      <c r="I16" s="100" t="s">
-        <v>119</v>
+      <c r="D16" s="94"/>
+      <c r="E16" s="95"/>
+      <c r="F16" s="96" t="s">
+        <v>103</v>
+      </c>
+      <c r="G16" s="97" t="s">
+        <v>125</v>
+      </c>
+      <c r="H16" s="98"/>
+      <c r="I16" s="99" t="s">
+        <v>120</v>
+      </c>
+      <c r="J16" s="100" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="101"/>
       <c r="B17" s="60" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C17" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="102"/>
-      <c r="E17" s="84" t="s">
-        <v>102</v>
-      </c>
-      <c r="F17" s="103" t="s">
-        <v>125</v>
-      </c>
-      <c r="G17" s="78"/>
-      <c r="H17" s="103"/>
-      <c r="I17" s="104"/>
+      <c r="D17" s="84"/>
+      <c r="E17" s="102"/>
+      <c r="F17" s="84" t="s">
+        <v>103</v>
+      </c>
+      <c r="G17" s="103" t="s">
+        <v>127</v>
+      </c>
+      <c r="H17" s="78"/>
+      <c r="I17" s="103"/>
+      <c r="J17" s="104"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="65"/>
       <c r="B18" s="105" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C18" s="106" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="107"/>
-      <c r="E18" s="67" t="s">
-        <v>102</v>
-      </c>
-      <c r="F18" s="69" t="s">
-        <v>127</v>
-      </c>
-      <c r="G18" s="108"/>
-      <c r="H18" s="69"/>
-      <c r="I18" s="109"/>
+      <c r="D18" s="106"/>
+      <c r="E18" s="107"/>
+      <c r="F18" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="G18" s="69" t="s">
+        <v>129</v>
+      </c>
+      <c r="H18" s="108"/>
+      <c r="I18" s="69"/>
+      <c r="J18" s="109"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="65"/>
       <c r="B19" s="105" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C19" s="106" t="s">
         <v>53</v>
       </c>
-      <c r="D19" s="107"/>
-      <c r="E19" s="67" t="s">
-        <v>102</v>
-      </c>
-      <c r="F19" s="69" t="s">
-        <v>129</v>
-      </c>
-      <c r="G19" s="108"/>
-      <c r="H19" s="69"/>
-      <c r="I19" s="109"/>
+      <c r="D19" s="106"/>
+      <c r="E19" s="107"/>
+      <c r="F19" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="G19" s="69" t="s">
+        <v>131</v>
+      </c>
+      <c r="H19" s="108"/>
+      <c r="I19" s="69"/>
+      <c r="J19" s="109"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="92"/>
       <c r="B20" s="93" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C20" s="94" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="110"/>
-      <c r="E20" s="96" t="s">
-        <v>102</v>
-      </c>
-      <c r="F20" s="97" t="s">
-        <v>131</v>
-      </c>
-      <c r="G20" s="111"/>
-      <c r="H20" s="97"/>
-      <c r="I20" s="112"/>
+      <c r="D20" s="94"/>
+      <c r="E20" s="110"/>
+      <c r="F20" s="96" t="s">
+        <v>103</v>
+      </c>
+      <c r="G20" s="97" t="s">
+        <v>133</v>
+      </c>
+      <c r="H20" s="111"/>
+      <c r="I20" s="97"/>
+      <c r="J20" s="112"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -6573,7 +6605,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="3:3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6592,10 +6624,10 @@
       <c r="C1" s="51"/>
       <c r="D1" s="51"/>
       <c r="E1" s="56" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F1" s="57" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6604,304 +6636,304 @@
       <c r="C2" s="116"/>
       <c r="D2" s="54"/>
       <c r="E2" s="117" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F2" s="118" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="119" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B3" s="119" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C3" s="117" t="s">
         <v>93</v>
       </c>
       <c r="D3" s="117" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E3" s="56" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="F3" s="57" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="120" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B4" s="121" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C4" s="60" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D4" s="62" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E4" s="122"/>
       <c r="F4" s="62"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="123" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B5" s="124" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C5" s="66" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D5" s="72" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E5" s="125"/>
       <c r="F5" s="72"/>
     </row>
     <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="123" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B6" s="124" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C6" s="66" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D6" s="72" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E6" s="125"/>
       <c r="F6" s="72"/>
     </row>
     <row r="7" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="123" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B7" s="124" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C7" s="66" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D7" s="72" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E7" s="125" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="F7" s="72"/>
     </row>
     <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="123" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B8" s="124" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C8" s="66" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D8" s="72" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E8" s="126"/>
       <c r="F8" s="74"/>
     </row>
     <row r="9" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="123" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B9" s="124" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C9" s="66" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D9" s="72" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E9" s="126"/>
       <c r="F9" s="74"/>
     </row>
     <row r="10" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="123" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B10" s="124" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C10" s="66" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D10" s="72" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E10" s="127"/>
       <c r="F10" s="72"/>
     </row>
     <row r="11" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="123" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B11" s="124" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C11" s="66" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D11" s="72" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E11" s="127"/>
       <c r="F11" s="72"/>
     </row>
     <row r="12" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="123" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B12" s="124" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C12" s="66" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D12" s="72" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E12" s="127"/>
       <c r="F12" s="72"/>
     </row>
     <row r="13" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="128" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B13" s="129" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C13" s="130" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D13" s="131" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E13" s="132" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="F13" s="133"/>
     </row>
     <row r="14" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="134" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B14" s="121" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C14" s="120" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D14" s="60" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E14" s="122"/>
       <c r="F14" s="62"/>
     </row>
     <row r="15" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="135" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B15" s="124" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C15" s="66" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D15" s="72" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E15" s="127"/>
       <c r="F15" s="136"/>
     </row>
     <row r="16" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="137" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B16" s="129" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C16" s="93" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D16" s="138" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E16" s="132"/>
       <c r="F16" s="133"/>
     </row>
     <row r="17" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="134" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B17" s="121" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C17" s="139" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D17" s="60" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E17" s="122"/>
       <c r="F17" s="62"/>
     </row>
     <row r="18" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="135" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B18" s="124" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C18" s="105" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D18" s="66" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E18" s="127"/>
       <c r="F18" s="136"/>
     </row>
     <row r="19" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="135" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B19" s="124" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C19" s="105" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D19" s="66" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E19" s="127"/>
       <c r="F19" s="72"/>
     </row>
     <row r="20" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="137" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B20" s="129" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C20" s="93" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D20" s="138" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E20" s="132"/>
       <c r="F20" s="133"/>
@@ -6925,8 +6957,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="3:3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6945,10 +6977,10 @@
       <c r="C1" s="51"/>
       <c r="D1" s="51"/>
       <c r="E1" s="140" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="F1" s="141" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6957,304 +6989,304 @@
       <c r="C2" s="116"/>
       <c r="D2" s="54"/>
       <c r="E2" s="142" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F2" s="143" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="119" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B3" s="119" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C3" s="117" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D3" s="117" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E3" s="56" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F3" s="57" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="120" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B4" s="144" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C4" s="60" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D4" s="62" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E4" s="122"/>
       <c r="F4" s="62"/>
     </row>
     <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="123" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B5" s="145" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C5" s="66" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D5" s="72" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E5" s="125"/>
       <c r="F5" s="72"/>
     </row>
     <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="123" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B6" s="145" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C6" s="66" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D6" s="146" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E6" s="125"/>
       <c r="F6" s="72"/>
     </row>
     <row r="7" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="123" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B7" s="145" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C7" s="66" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D7" s="146" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E7" s="125" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="F7" s="72"/>
     </row>
     <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="123" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B8" s="145" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C8" s="66" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D8" s="146" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E8" s="126"/>
       <c r="F8" s="74"/>
     </row>
     <row r="9" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="123" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B9" s="145" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C9" s="66" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D9" s="146" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E9" s="126"/>
       <c r="F9" s="74"/>
     </row>
     <row r="10" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="123" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B10" s="145" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C10" s="66" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D10" s="146" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="E10" s="127"/>
       <c r="F10" s="72"/>
     </row>
     <row r="11" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="123" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B11" s="145" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C11" s="66" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D11" s="146" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E11" s="127"/>
       <c r="F11" s="72"/>
     </row>
     <row r="12" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="123" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B12" s="145" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C12" s="66" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D12" s="146" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E12" s="127"/>
       <c r="F12" s="72"/>
     </row>
     <row r="13" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="128" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B13" s="147" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C13" s="130" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D13" s="131" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E13" s="132" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="F13" s="133"/>
     </row>
     <row r="14" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="134" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B14" s="144" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C14" s="120" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D14" s="148" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E14" s="122"/>
       <c r="F14" s="62"/>
     </row>
     <row r="15" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="135" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B15" s="145" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C15" s="66" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D15" s="146" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E15" s="127"/>
       <c r="F15" s="136"/>
     </row>
     <row r="16" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="137" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B16" s="147" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C16" s="93" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D16" s="149" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E16" s="132"/>
       <c r="F16" s="133"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="134" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B17" s="144" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C17" s="139" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D17" s="148" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="E17" s="122"/>
       <c r="F17" s="62"/>
     </row>
     <row r="18" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="135" t="s">
+        <v>196</v>
+      </c>
+      <c r="B18" s="145" t="s">
         <v>194</v>
       </c>
-      <c r="B18" s="145" t="s">
-        <v>192</v>
-      </c>
       <c r="C18" s="105" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D18" s="150" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="E18" s="127"/>
       <c r="F18" s="136"/>
     </row>
     <row r="19" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="135" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B19" s="145" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C19" s="105" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D19" s="150" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E19" s="127"/>
       <c r="F19" s="72"/>
     </row>
     <row r="20" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="137" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B20" s="147" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C20" s="93" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D20" s="149" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="E20" s="132"/>
       <c r="F20" s="133"/>

</xml_diff>